<commit_message>
Updated Gantt and personal scripts
</commit_message>
<xml_diff>
--- a/Docs/Group/Team_Gantt_Chart.xlsx
+++ b/Docs/Group/Team_Gantt_Chart.xlsx
@@ -5,13 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Brandon Foss\Documents\GitHub\6_Angry_Devs\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Brandon Foss\Documents\GitHub\6_Angry_Devs\Docs\Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8274FBA-AB16-4826-B44E-4ABCE6694D82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9647F7-9D8C-456D-9219-8F371FB6901C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17625" xr2:uid="{12D7657A-059A-4288-9760-83C71639AA7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="3" r:id="rId1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="99">
   <si>
     <t>testing</t>
   </si>
@@ -322,6 +321,15 @@
   </si>
   <si>
     <t>Apr. 8</t>
+  </si>
+  <si>
+    <t>ship spawn assurance</t>
+  </si>
+  <si>
+    <t>Oral Exam Prep</t>
+  </si>
+  <si>
+    <t>Apr. 14</t>
   </si>
 </sst>
 </file>
@@ -1309,10 +1317,7 @@
   <dimension ref="B1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,39 +1408,39 @@
       </c>
       <c r="C4" s="20">
         <f t="shared" ref="C4:D9" si="0">(G4+K4 +O4)</f>
-        <v>7000</v>
+        <v>7200</v>
       </c>
       <c r="D4" s="21">
         <f t="shared" si="0"/>
-        <v>6550</v>
+        <v>8050</v>
       </c>
       <c r="E4" s="22">
         <f t="shared" ref="E4:E9" si="1">(C4-D4)</f>
-        <v>450</v>
+        <v>-850</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="14">
-        <f>(Gantt!$B10)*100</f>
-        <v>3700</v>
+        <f>(Gantt!$B11)*100</f>
+        <v>3900</v>
       </c>
       <c r="H4" s="15">
-        <f>(Gantt!$C10)*100</f>
-        <v>3600</v>
+        <f>(Gantt!$C11)*100</f>
+        <v>4900</v>
       </c>
       <c r="I4" s="16">
         <f t="shared" ref="I4:I9" si="2">(G4-H4)</f>
-        <v>100</v>
+        <v>-1000</v>
       </c>
       <c r="K4" s="110">
         <v>2000</v>
       </c>
       <c r="L4" s="21">
         <f>Meetings!B4*100</f>
-        <v>1650</v>
+        <v>1850</v>
       </c>
       <c r="M4" s="22">
         <f t="shared" ref="M4:M9" si="3">(K4-L4)</f>
-        <v>350</v>
+        <v>150</v>
       </c>
       <c r="O4" s="47">
         <f>(SA!C7)*100</f>
@@ -1456,39 +1461,39 @@
       </c>
       <c r="C5" s="14">
         <f t="shared" si="0"/>
-        <v>13200</v>
+        <v>13900</v>
       </c>
       <c r="D5" s="15">
         <f t="shared" si="0"/>
-        <v>8750</v>
+        <v>10350</v>
       </c>
       <c r="E5" s="16">
         <f t="shared" si="1"/>
-        <v>4450</v>
+        <v>3550</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="14">
-        <f>(Gantt!$B20)*100</f>
-        <v>10000</v>
+        <f>(Gantt!$B22)*100</f>
+        <v>10700</v>
       </c>
       <c r="H5" s="15">
-        <f>(Gantt!$C20)*100</f>
-        <v>5900</v>
+        <f>(Gantt!$C22)*100</f>
+        <v>7300</v>
       </c>
       <c r="I5" s="16">
         <f t="shared" si="2"/>
-        <v>4100</v>
+        <v>3400</v>
       </c>
       <c r="K5" s="112">
         <v>2000</v>
       </c>
       <c r="L5" s="15">
         <f>Meetings!B5*100</f>
-        <v>1650</v>
+        <v>1850</v>
       </c>
       <c r="M5" s="16">
         <f t="shared" si="3"/>
-        <v>350</v>
+        <v>150</v>
       </c>
       <c r="O5" s="44">
         <f>(SA!C12)*100</f>
@@ -1513,35 +1518,35 @@
       </c>
       <c r="D6" s="15">
         <f t="shared" si="0"/>
-        <v>4850</v>
+        <v>5650</v>
       </c>
       <c r="E6" s="16">
         <f t="shared" si="1"/>
-        <v>1950</v>
+        <v>1150</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="14">
-        <f>(Gantt!$B29)*100</f>
+        <f>(Gantt!$B31)*100</f>
         <v>3600</v>
       </c>
       <c r="H6" s="15">
-        <f>(Gantt!$C29)*100</f>
-        <v>2600</v>
+        <f>(Gantt!$C31)*100</f>
+        <v>3200</v>
       </c>
       <c r="I6" s="16">
         <f t="shared" si="2"/>
-        <v>1000</v>
+        <v>400</v>
       </c>
       <c r="K6" s="112">
         <v>2000</v>
       </c>
       <c r="L6" s="15">
         <f>Meetings!B6*100</f>
-        <v>1150</v>
+        <v>1350</v>
       </c>
       <c r="M6" s="16">
         <f t="shared" si="3"/>
-        <v>850</v>
+        <v>650</v>
       </c>
       <c r="N6" s="42"/>
       <c r="O6" s="45">
@@ -1567,35 +1572,35 @@
       </c>
       <c r="D7" s="45">
         <f t="shared" si="0"/>
-        <v>6400</v>
+        <v>6800</v>
       </c>
       <c r="E7" s="46">
         <f t="shared" si="1"/>
-        <v>300</v>
+        <v>-100</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="14">
-        <f>(Gantt!$B38)*100</f>
+        <f>(Gantt!$B40)*100</f>
         <v>3500</v>
       </c>
       <c r="H7" s="15">
-        <f>(Gantt!$C38)*100</f>
-        <v>3800</v>
+        <f>(Gantt!$C40)*100</f>
+        <v>4000</v>
       </c>
       <c r="I7" s="16">
         <f t="shared" si="2"/>
-        <v>-300</v>
+        <v>-500</v>
       </c>
       <c r="K7" s="112">
         <v>2000</v>
       </c>
       <c r="L7" s="15">
         <f>Meetings!B7*100</f>
-        <v>1500</v>
+        <v>1700</v>
       </c>
       <c r="M7" s="16">
         <f t="shared" si="3"/>
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="N7" s="42"/>
       <c r="O7" s="56">
@@ -1621,35 +1626,35 @@
       </c>
       <c r="D8" s="45">
         <f t="shared" si="0"/>
-        <v>5050</v>
+        <v>7250</v>
       </c>
       <c r="E8" s="46">
         <f t="shared" si="1"/>
-        <v>4250</v>
+        <v>2050</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="14">
-        <f>(Gantt!$B46)*100</f>
+        <f>(Gantt!$B48)*100</f>
         <v>6100</v>
       </c>
       <c r="H8" s="15">
-        <f>(Gantt!$C46)*100</f>
-        <v>2900</v>
+        <f>(Gantt!$C48)*100</f>
+        <v>4900</v>
       </c>
       <c r="I8" s="16">
         <f t="shared" si="2"/>
-        <v>3200</v>
+        <v>1200</v>
       </c>
       <c r="K8" s="112">
         <v>2000</v>
       </c>
       <c r="L8" s="15">
         <f>Meetings!B8*100</f>
-        <v>950</v>
+        <v>1150</v>
       </c>
       <c r="M8" s="16">
         <f t="shared" si="3"/>
-        <v>1050</v>
+        <v>850</v>
       </c>
       <c r="N8" s="42"/>
       <c r="O8" s="56">
@@ -1682,11 +1687,11 @@
         <v>3250</v>
       </c>
       <c r="G9" s="14">
-        <f>(Gantt!$B54)*100</f>
+        <f>(Gantt!$B56)*100</f>
         <v>2200</v>
       </c>
       <c r="H9" s="15">
-        <f>(Gantt!$C54)*100</f>
+        <f>(Gantt!$C56)*100</f>
         <v>1200</v>
       </c>
       <c r="I9" s="16">
@@ -1723,27 +1728,27 @@
       </c>
       <c r="C10" s="24">
         <f>SUM(C4:C9)</f>
-        <v>48400</v>
+        <v>49300</v>
       </c>
       <c r="D10" s="25">
         <f>SUM(D4:D9)</f>
-        <v>33750</v>
+        <v>40250</v>
       </c>
       <c r="E10" s="26">
         <f>SUM(E4:E9)</f>
-        <v>14650</v>
+        <v>9050</v>
       </c>
       <c r="G10" s="17">
         <f>SUM(G4:G9)</f>
-        <v>29100</v>
+        <v>30000</v>
       </c>
       <c r="H10" s="18">
         <f>SUM(H4:H9)</f>
-        <v>20000</v>
+        <v>25500</v>
       </c>
       <c r="I10" s="19">
         <f>SUM(I4:I9)</f>
-        <v>9100</v>
+        <v>4500</v>
       </c>
       <c r="K10" s="17">
         <f>SUM(K4:K9)</f>
@@ -1751,11 +1756,11 @@
       </c>
       <c r="L10" s="18">
         <f>SUM(L4:L9)</f>
-        <v>7450</v>
+        <v>8450</v>
       </c>
       <c r="M10" s="19">
         <f>SUM(M4:M9)</f>
-        <v>4550</v>
+        <v>3550</v>
       </c>
       <c r="O10" s="24">
         <f>SUM(O4:O9)</f>
@@ -1787,11 +1792,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AZ66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="S58" sqref="S58"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1957,8 +1959,12 @@
       <c r="AS2" s="90">
         <v>123</v>
       </c>
-      <c r="AT2" s="43"/>
-      <c r="AU2" s="43"/>
+      <c r="AT2" s="90">
+        <v>125</v>
+      </c>
+      <c r="AU2" s="90">
+        <v>128</v>
+      </c>
       <c r="AV2" s="43"/>
       <c r="AW2" s="43"/>
       <c r="AX2" s="43"/>
@@ -1973,7 +1979,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="69">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" s="51"/>
       <c r="E3" s="93"/>
@@ -2008,9 +2014,9 @@
       <c r="AP3" s="43"/>
       <c r="AQ3" s="43"/>
       <c r="AR3" s="43"/>
-      <c r="AS3" s="106"/>
+      <c r="AS3" s="43"/>
       <c r="AT3" s="43"/>
-      <c r="AU3" s="43"/>
+      <c r="AU3" s="106"/>
       <c r="AV3" s="43"/>
       <c r="AW3" s="43"/>
       <c r="AX3" s="43"/>
@@ -2025,14 +2031,14 @@
         <v>6</v>
       </c>
       <c r="C4" s="69">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="51"/>
       <c r="E4" s="51"/>
       <c r="F4" s="93"/>
       <c r="G4" s="93"/>
       <c r="H4" s="93"/>
-      <c r="I4" s="103"/>
+      <c r="I4" s="93"/>
       <c r="J4" s="51"/>
       <c r="K4" s="51"/>
       <c r="L4" s="51"/>
@@ -2060,9 +2066,9 @@
       <c r="AP4" s="43"/>
       <c r="AQ4" s="43"/>
       <c r="AR4" s="43"/>
-      <c r="AS4" s="107"/>
+      <c r="AS4" s="43"/>
       <c r="AT4" s="43"/>
-      <c r="AU4" s="43"/>
+      <c r="AU4" s="107"/>
       <c r="AV4" s="43"/>
       <c r="AW4" s="43"/>
       <c r="AX4" s="43"/>
@@ -2077,7 +2083,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="69">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D5" s="51"/>
       <c r="E5" s="51"/>
@@ -2112,9 +2118,9 @@
       <c r="AP5" s="43"/>
       <c r="AQ5" s="43"/>
       <c r="AR5" s="43"/>
-      <c r="AS5" s="107"/>
+      <c r="AS5" s="43"/>
       <c r="AT5" s="43"/>
-      <c r="AU5" s="43"/>
+      <c r="AU5" s="107"/>
       <c r="AV5" s="43"/>
       <c r="AW5" s="43"/>
       <c r="AX5" s="43"/>
@@ -2129,7 +2135,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="69">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D6" s="51"/>
       <c r="E6" s="51"/>
@@ -2141,7 +2147,7 @@
       <c r="K6" s="51"/>
       <c r="L6" s="93"/>
       <c r="M6" s="93"/>
-      <c r="N6" s="51"/>
+      <c r="N6" s="93"/>
       <c r="O6" s="51"/>
       <c r="P6" s="51"/>
       <c r="Q6" s="51"/>
@@ -2164,9 +2170,9 @@
       <c r="AP6" s="43"/>
       <c r="AQ6" s="43"/>
       <c r="AR6" s="43"/>
-      <c r="AS6" s="107"/>
+      <c r="AS6" s="43"/>
       <c r="AT6" s="43"/>
-      <c r="AU6" s="43"/>
+      <c r="AU6" s="107"/>
       <c r="AV6" s="43"/>
       <c r="AW6" s="43"/>
       <c r="AX6" s="43"/>
@@ -2193,8 +2199,8 @@
       <c r="K7" s="51"/>
       <c r="L7" s="51"/>
       <c r="M7" s="51"/>
-      <c r="N7" s="93"/>
-      <c r="O7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="93"/>
       <c r="P7" s="51"/>
       <c r="Q7" s="51"/>
       <c r="R7" s="51"/>
@@ -2216,9 +2222,9 @@
       <c r="AP7" s="43"/>
       <c r="AQ7" s="43"/>
       <c r="AR7" s="43"/>
-      <c r="AS7" s="107"/>
+      <c r="AS7" s="43"/>
       <c r="AT7" s="43"/>
-      <c r="AU7" s="43"/>
+      <c r="AU7" s="107"/>
       <c r="AV7" s="43"/>
       <c r="AW7" s="43"/>
       <c r="AX7" s="43"/>
@@ -2233,7 +2239,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="69">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D8" s="51"/>
       <c r="E8" s="51"/>
@@ -2246,11 +2252,11 @@
       <c r="L8" s="51"/>
       <c r="M8" s="51"/>
       <c r="N8" s="51"/>
-      <c r="O8" s="93"/>
+      <c r="O8" s="51"/>
       <c r="P8" s="93"/>
-      <c r="Q8" s="103"/>
-      <c r="R8" s="51"/>
-      <c r="S8" s="51"/>
+      <c r="Q8" s="93"/>
+      <c r="R8" s="93"/>
+      <c r="S8" s="103"/>
       <c r="T8" s="51"/>
       <c r="U8" s="51"/>
       <c r="V8" s="51"/>
@@ -2268,9 +2274,9 @@
       <c r="AP8" s="43"/>
       <c r="AQ8" s="43"/>
       <c r="AR8" s="43"/>
-      <c r="AS8" s="107"/>
+      <c r="AS8" s="43"/>
       <c r="AT8" s="43"/>
-      <c r="AU8" s="43"/>
+      <c r="AU8" s="107"/>
       <c r="AV8" s="43"/>
       <c r="AW8" s="43"/>
       <c r="AX8" s="43"/>
@@ -2279,13 +2285,13 @@
     </row>
     <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="92" t="s">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="B9" s="69">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="69">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D9" s="51"/>
       <c r="E9" s="51"/>
@@ -2301,9 +2307,9 @@
       <c r="O9" s="51"/>
       <c r="P9" s="51"/>
       <c r="Q9" s="51"/>
-      <c r="R9" s="93"/>
-      <c r="S9" s="93"/>
-      <c r="T9" s="94"/>
+      <c r="R9" s="51"/>
+      <c r="S9" s="51"/>
+      <c r="T9" s="93"/>
       <c r="U9" s="51"/>
       <c r="V9" s="51"/>
       <c r="W9" s="51"/>
@@ -2320,119 +2326,131 @@
       <c r="AP9" s="43"/>
       <c r="AQ9" s="43"/>
       <c r="AR9" s="43"/>
-      <c r="AS9" s="107"/>
+      <c r="AS9" s="43"/>
       <c r="AT9" s="43"/>
-      <c r="AU9" s="43"/>
+      <c r="AU9" s="107"/>
       <c r="AV9" s="43"/>
       <c r="AW9" s="43"/>
       <c r="AX9" s="43"/>
       <c r="AY9" s="43"/>
       <c r="AZ9" s="43"/>
     </row>
-    <row r="10" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="95">
-        <f>SUM(B3:B9)</f>
-        <v>37</v>
-      </c>
-      <c r="C10" s="95">
-        <f>SUM(C3:C9)</f>
-        <v>36</v>
-      </c>
-      <c r="D10" s="96"/>
-      <c r="E10" s="96"/>
-      <c r="F10" s="96"/>
-      <c r="G10" s="96"/>
-      <c r="H10" s="96"/>
-      <c r="I10" s="96"/>
-      <c r="J10" s="96"/>
-      <c r="K10" s="96"/>
-      <c r="L10" s="96"/>
-      <c r="M10" s="96"/>
-      <c r="N10" s="96"/>
-      <c r="O10" s="96"/>
-      <c r="P10" s="96"/>
-      <c r="Q10" s="96"/>
-      <c r="R10" s="96"/>
-      <c r="S10" s="96"/>
-      <c r="T10" s="96"/>
-      <c r="U10" s="96"/>
-      <c r="V10" s="96"/>
-      <c r="W10" s="96"/>
-      <c r="X10" s="96"/>
-      <c r="Y10" s="96"/>
-      <c r="Z10" s="96"/>
-      <c r="AA10" s="96"/>
-      <c r="AB10" s="96"/>
-      <c r="AC10" s="96"/>
-      <c r="AD10" s="96"/>
-      <c r="AE10" s="96"/>
-      <c r="AF10" s="96"/>
-      <c r="AG10" s="96"/>
-      <c r="AH10" s="96"/>
-      <c r="AI10" s="96"/>
-      <c r="AJ10" s="96"/>
-      <c r="AK10" s="96"/>
-      <c r="AL10" s="96"/>
-      <c r="AM10" s="96"/>
-      <c r="AN10" s="96"/>
-      <c r="AO10" s="96"/>
-      <c r="AP10" s="96"/>
-      <c r="AQ10" s="96"/>
-      <c r="AR10" s="96"/>
-      <c r="AS10" s="108"/>
+    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A10" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="69">
+        <v>3</v>
+      </c>
+      <c r="C10" s="69">
+        <v>7</v>
+      </c>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="51"/>
+      <c r="S10" s="51"/>
+      <c r="T10" s="51"/>
+      <c r="U10" s="93"/>
+      <c r="V10" s="93"/>
+      <c r="W10" s="103"/>
+      <c r="X10" s="51"/>
+      <c r="Y10" s="51"/>
+      <c r="Z10" s="51"/>
+      <c r="AA10" s="51"/>
+      <c r="AB10" s="51"/>
+      <c r="AC10" s="51"/>
+      <c r="AD10" s="51"/>
+      <c r="AE10" s="51"/>
+      <c r="AF10" s="43"/>
+      <c r="AG10" s="43"/>
+      <c r="AH10" s="43"/>
+      <c r="AI10" s="43"/>
+      <c r="AJ10" s="43"/>
+      <c r="AK10" s="43"/>
+      <c r="AL10" s="43"/>
+      <c r="AM10" s="43"/>
+      <c r="AN10" s="43"/>
+      <c r="AO10" s="43"/>
+      <c r="AP10" s="43"/>
+      <c r="AQ10" s="43"/>
+      <c r="AR10" s="43"/>
+      <c r="AS10" s="43"/>
       <c r="AT10" s="43"/>
-      <c r="AU10" s="43"/>
+      <c r="AU10" s="107"/>
       <c r="AV10" s="43"/>
       <c r="AW10" s="43"/>
       <c r="AX10" s="43"/>
       <c r="AY10" s="43"/>
       <c r="AZ10" s="43"/>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A11" s="98" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="88"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="60"/>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="60"/>
-      <c r="O11" s="60"/>
-      <c r="P11" s="60"/>
-      <c r="Q11" s="60"/>
-      <c r="R11" s="60"/>
-      <c r="S11" s="60"/>
-      <c r="T11" s="60"/>
-      <c r="U11" s="60"/>
-      <c r="V11" s="60"/>
-      <c r="W11" s="60"/>
-      <c r="X11" s="60"/>
-      <c r="Y11" s="60"/>
-      <c r="Z11" s="60"/>
-      <c r="AA11" s="60"/>
-      <c r="AB11" s="60"/>
-      <c r="AC11" s="60"/>
-      <c r="AD11" s="60"/>
-      <c r="AE11" s="60"/>
-      <c r="AN11" s="43"/>
-      <c r="AO11" s="43"/>
-      <c r="AP11" s="43"/>
-      <c r="AQ11" s="43"/>
-      <c r="AR11" s="43"/>
-      <c r="AS11" s="107"/>
-      <c r="AT11" s="43"/>
-      <c r="AU11" s="43"/>
+    <row r="11" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="95">
+        <f>SUM(B3:B10)</f>
+        <v>39</v>
+      </c>
+      <c r="C11" s="95">
+        <f>SUM(C3:C10)</f>
+        <v>49</v>
+      </c>
+      <c r="D11" s="96"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="96"/>
+      <c r="G11" s="96"/>
+      <c r="H11" s="96"/>
+      <c r="I11" s="96"/>
+      <c r="J11" s="96"/>
+      <c r="K11" s="96"/>
+      <c r="L11" s="96"/>
+      <c r="M11" s="96"/>
+      <c r="N11" s="96"/>
+      <c r="O11" s="96"/>
+      <c r="P11" s="96"/>
+      <c r="Q11" s="96"/>
+      <c r="R11" s="96"/>
+      <c r="S11" s="96"/>
+      <c r="T11" s="96"/>
+      <c r="U11" s="96"/>
+      <c r="V11" s="96"/>
+      <c r="W11" s="96"/>
+      <c r="X11" s="96"/>
+      <c r="Y11" s="96"/>
+      <c r="Z11" s="96"/>
+      <c r="AA11" s="96"/>
+      <c r="AB11" s="96"/>
+      <c r="AC11" s="96"/>
+      <c r="AD11" s="96"/>
+      <c r="AE11" s="96"/>
+      <c r="AF11" s="96"/>
+      <c r="AG11" s="96"/>
+      <c r="AH11" s="96"/>
+      <c r="AI11" s="96"/>
+      <c r="AJ11" s="96"/>
+      <c r="AK11" s="96"/>
+      <c r="AL11" s="96"/>
+      <c r="AM11" s="96"/>
+      <c r="AN11" s="96"/>
+      <c r="AO11" s="96"/>
+      <c r="AP11" s="96"/>
+      <c r="AQ11" s="96"/>
+      <c r="AR11" s="96"/>
+      <c r="AS11" s="96"/>
+      <c r="AT11" s="96"/>
+      <c r="AU11" s="108"/>
       <c r="AV11" s="43"/>
       <c r="AW11" s="43"/>
       <c r="AX11" s="43"/>
@@ -2440,51 +2458,47 @@
       <c r="AZ11" s="43"/>
     </row>
     <row r="12" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A12" s="92" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="69">
-        <v>3</v>
-      </c>
-      <c r="C12" s="69">
-        <v>2</v>
-      </c>
-      <c r="D12" s="51"/>
-      <c r="E12" s="102"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="51"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="51"/>
-      <c r="K12" s="51"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="51"/>
-      <c r="N12" s="51"/>
-      <c r="O12" s="51"/>
-      <c r="P12" s="51"/>
-      <c r="Q12" s="51"/>
-      <c r="R12" s="51"/>
-      <c r="S12" s="51"/>
-      <c r="T12" s="51"/>
-      <c r="U12" s="51"/>
-      <c r="V12" s="51"/>
-      <c r="W12" s="51"/>
-      <c r="X12" s="51"/>
-      <c r="Y12" s="51"/>
-      <c r="Z12" s="51"/>
-      <c r="AA12" s="51"/>
-      <c r="AB12" s="51"/>
-      <c r="AC12" s="51"/>
-      <c r="AD12" s="51"/>
-      <c r="AE12" s="51"/>
+      <c r="A12" s="98" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="88"/>
+      <c r="C12" s="88"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="60"/>
+      <c r="P12" s="60"/>
+      <c r="Q12" s="60"/>
+      <c r="R12" s="60"/>
+      <c r="S12" s="60"/>
+      <c r="T12" s="60"/>
+      <c r="U12" s="60"/>
+      <c r="V12" s="60"/>
+      <c r="W12" s="60"/>
+      <c r="X12" s="60"/>
+      <c r="Y12" s="60"/>
+      <c r="Z12" s="60"/>
+      <c r="AA12" s="60"/>
+      <c r="AB12" s="60"/>
+      <c r="AC12" s="60"/>
+      <c r="AD12" s="60"/>
+      <c r="AE12" s="60"/>
       <c r="AN12" s="43"/>
       <c r="AO12" s="43"/>
       <c r="AP12" s="43"/>
       <c r="AQ12" s="43"/>
       <c r="AR12" s="43"/>
-      <c r="AS12" s="107"/>
+      <c r="AS12" s="43"/>
       <c r="AT12" s="43"/>
-      <c r="AU12" s="43"/>
+      <c r="AU12" s="107"/>
       <c r="AV12" s="43"/>
       <c r="AW12" s="43"/>
       <c r="AX12" s="43"/>
@@ -2493,21 +2507,21 @@
     </row>
     <row r="13" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A13" s="92" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B13" s="69">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C13" s="69">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="93"/>
-      <c r="G13" s="93"/>
-      <c r="H13" s="93"/>
-      <c r="I13" s="93"/>
-      <c r="J13" s="93"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="51"/>
       <c r="K13" s="51"/>
       <c r="L13" s="51"/>
       <c r="M13" s="51"/>
@@ -2534,9 +2548,9 @@
       <c r="AP13" s="43"/>
       <c r="AQ13" s="43"/>
       <c r="AR13" s="43"/>
-      <c r="AS13" s="107"/>
+      <c r="AS13" s="43"/>
       <c r="AT13" s="43"/>
-      <c r="AU13" s="43"/>
+      <c r="AU13" s="107"/>
       <c r="AV13" s="43"/>
       <c r="AW13" s="43"/>
       <c r="AX13" s="43"/>
@@ -2545,25 +2559,25 @@
     </row>
     <row r="14" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A14" s="92" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B14" s="69">
         <v>5</v>
       </c>
       <c r="C14" s="69">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D14" s="51"/>
       <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="59"/>
-      <c r="K14" s="93"/>
-      <c r="L14" s="93"/>
-      <c r="M14" s="93"/>
-      <c r="N14" s="93"/>
+      <c r="F14" s="93"/>
+      <c r="G14" s="93"/>
+      <c r="H14" s="93"/>
+      <c r="I14" s="93"/>
+      <c r="J14" s="93"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
       <c r="O14" s="51"/>
       <c r="P14" s="51"/>
       <c r="Q14" s="51"/>
@@ -2586,9 +2600,9 @@
       <c r="AP14" s="43"/>
       <c r="AQ14" s="43"/>
       <c r="AR14" s="43"/>
-      <c r="AS14" s="107"/>
+      <c r="AS14" s="43"/>
       <c r="AT14" s="43"/>
-      <c r="AU14" s="43"/>
+      <c r="AU14" s="107"/>
       <c r="AV14" s="43"/>
       <c r="AW14" s="43"/>
       <c r="AX14" s="43"/>
@@ -2597,35 +2611,35 @@
     </row>
     <row r="15" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A15" s="92" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B15" s="69">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C15" s="69">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="51"/>
       <c r="E15" s="51"/>
       <c r="F15" s="51"/>
       <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="51"/>
-      <c r="L15" s="51"/>
-      <c r="M15" s="51"/>
-      <c r="N15" s="51"/>
-      <c r="O15" s="93"/>
-      <c r="P15" s="93"/>
-      <c r="Q15" s="93"/>
-      <c r="R15" s="93"/>
-      <c r="S15" s="93"/>
-      <c r="T15" s="103"/>
-      <c r="U15" s="94"/>
-      <c r="V15" s="94"/>
-      <c r="W15" s="94"/>
-      <c r="X15" s="94"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="93"/>
+      <c r="L15" s="93"/>
+      <c r="M15" s="93"/>
+      <c r="N15" s="93"/>
+      <c r="O15" s="51"/>
+      <c r="P15" s="51"/>
+      <c r="Q15" s="51"/>
+      <c r="R15" s="51"/>
+      <c r="S15" s="51"/>
+      <c r="T15" s="51"/>
+      <c r="U15" s="51"/>
+      <c r="V15" s="51"/>
+      <c r="W15" s="51"/>
+      <c r="X15" s="51"/>
       <c r="Y15" s="51"/>
       <c r="Z15" s="51"/>
       <c r="AA15" s="51"/>
@@ -2638,9 +2652,9 @@
       <c r="AP15" s="43"/>
       <c r="AQ15" s="43"/>
       <c r="AR15" s="43"/>
-      <c r="AS15" s="107"/>
+      <c r="AS15" s="43"/>
       <c r="AT15" s="43"/>
-      <c r="AU15" s="43"/>
+      <c r="AU15" s="107"/>
       <c r="AV15" s="43"/>
       <c r="AW15" s="43"/>
       <c r="AX15" s="43"/>
@@ -2649,13 +2663,13 @@
     </row>
     <row r="16" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A16" s="92" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" s="69">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C16" s="69">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D16" s="51"/>
       <c r="E16" s="51"/>
@@ -2668,31 +2682,31 @@
       <c r="L16" s="51"/>
       <c r="M16" s="51"/>
       <c r="N16" s="51"/>
-      <c r="O16" s="51"/>
-      <c r="P16" s="51"/>
-      <c r="Q16" s="51"/>
-      <c r="R16" s="51"/>
-      <c r="S16" s="51"/>
-      <c r="T16" s="51"/>
-      <c r="U16" s="51"/>
-      <c r="V16" s="51"/>
-      <c r="W16" s="51"/>
-      <c r="X16" s="51"/>
-      <c r="Y16" s="93"/>
-      <c r="Z16" s="93"/>
-      <c r="AA16" s="103"/>
-      <c r="AB16" s="94"/>
-      <c r="AC16" s="94"/>
-      <c r="AD16" s="94"/>
-      <c r="AE16" s="94"/>
+      <c r="O16" s="93"/>
+      <c r="P16" s="93"/>
+      <c r="Q16" s="93"/>
+      <c r="R16" s="93"/>
+      <c r="S16" s="93"/>
+      <c r="T16" s="103"/>
+      <c r="U16" s="94"/>
+      <c r="V16" s="94"/>
+      <c r="W16" s="94"/>
+      <c r="X16" s="94"/>
+      <c r="Y16" s="51"/>
+      <c r="Z16" s="51"/>
+      <c r="AA16" s="51"/>
+      <c r="AB16" s="51"/>
+      <c r="AC16" s="51"/>
+      <c r="AD16" s="51"/>
+      <c r="AE16" s="51"/>
       <c r="AN16" s="43"/>
       <c r="AO16" s="43"/>
       <c r="AP16" s="43"/>
       <c r="AQ16" s="43"/>
       <c r="AR16" s="43"/>
-      <c r="AS16" s="107"/>
+      <c r="AS16" s="43"/>
       <c r="AT16" s="43"/>
-      <c r="AU16" s="43"/>
+      <c r="AU16" s="107"/>
       <c r="AV16" s="43"/>
       <c r="AW16" s="43"/>
       <c r="AX16" s="43"/>
@@ -2701,13 +2715,13 @@
     </row>
     <row r="17" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A17" s="92" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="B17" s="69">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C17" s="69">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D17" s="51"/>
       <c r="E17" s="51"/>
@@ -2730,26 +2744,21 @@
       <c r="V17" s="51"/>
       <c r="W17" s="51"/>
       <c r="X17" s="51"/>
-      <c r="Y17" s="51"/>
-      <c r="Z17" s="51"/>
-      <c r="AA17" s="51"/>
-      <c r="AB17" s="51"/>
-      <c r="AC17" s="51"/>
-      <c r="AD17" s="51"/>
-      <c r="AE17" s="51"/>
-      <c r="AF17" s="104"/>
-      <c r="AG17" s="2"/>
-      <c r="AH17" s="4"/>
-      <c r="AI17" s="4"/>
-      <c r="AJ17" s="4"/>
+      <c r="Y17" s="93"/>
+      <c r="Z17" s="93"/>
+      <c r="AA17" s="103"/>
+      <c r="AB17" s="94"/>
+      <c r="AC17" s="94"/>
+      <c r="AD17" s="94"/>
+      <c r="AE17" s="94"/>
       <c r="AN17" s="43"/>
       <c r="AO17" s="43"/>
       <c r="AP17" s="43"/>
       <c r="AQ17" s="43"/>
       <c r="AR17" s="43"/>
-      <c r="AS17" s="107"/>
+      <c r="AS17" s="43"/>
       <c r="AT17" s="43"/>
-      <c r="AU17" s="43"/>
+      <c r="AU17" s="107"/>
       <c r="AV17" s="43"/>
       <c r="AW17" s="43"/>
       <c r="AX17" s="43"/>
@@ -2758,18 +2767,18 @@
     </row>
     <row r="18" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A18" s="92" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B18" s="69">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C18" s="69">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D18" s="51"/>
       <c r="E18" s="51"/>
       <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
+      <c r="G18" s="59"/>
       <c r="H18" s="51"/>
       <c r="I18" s="51"/>
       <c r="J18" s="51"/>
@@ -2794,17 +2803,19 @@
       <c r="AC18" s="51"/>
       <c r="AD18" s="51"/>
       <c r="AE18" s="51"/>
-      <c r="AK18" s="104"/>
-      <c r="AL18" s="2"/>
-      <c r="AM18" s="43"/>
+      <c r="AF18" s="104"/>
+      <c r="AG18" s="104"/>
+      <c r="AH18" s="2"/>
+      <c r="AI18" s="4"/>
+      <c r="AJ18" s="4"/>
       <c r="AN18" s="43"/>
       <c r="AO18" s="43"/>
       <c r="AP18" s="43"/>
       <c r="AQ18" s="43"/>
       <c r="AR18" s="43"/>
-      <c r="AS18" s="107"/>
+      <c r="AS18" s="43"/>
       <c r="AT18" s="43"/>
-      <c r="AU18" s="43"/>
+      <c r="AU18" s="107"/>
       <c r="AV18" s="43"/>
       <c r="AW18" s="43"/>
       <c r="AX18" s="43"/>
@@ -2813,18 +2824,18 @@
     </row>
     <row r="19" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A19" s="92" t="s">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="B19" s="69">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C19" s="69">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D19" s="51"/>
       <c r="E19" s="51"/>
       <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
+      <c r="G19" s="59"/>
       <c r="H19" s="51"/>
       <c r="I19" s="51"/>
       <c r="J19" s="51"/>
@@ -2849,79 +2860,77 @@
       <c r="AC19" s="51"/>
       <c r="AD19" s="51"/>
       <c r="AE19" s="51"/>
-      <c r="AK19" s="43"/>
-      <c r="AL19" s="43"/>
-      <c r="AM19" s="104"/>
-      <c r="AN19" s="4"/>
-      <c r="AO19" s="4"/>
-      <c r="AP19" s="4"/>
-      <c r="AQ19" s="4"/>
-      <c r="AR19" s="4"/>
-      <c r="AS19" s="109"/>
+      <c r="AF19" s="51"/>
+      <c r="AG19" s="51"/>
+      <c r="AH19" s="51"/>
+      <c r="AI19" s="51"/>
+      <c r="AJ19" s="51"/>
+      <c r="AK19" s="104"/>
+      <c r="AL19" s="104"/>
+      <c r="AM19" s="2"/>
+      <c r="AN19" s="43"/>
+      <c r="AO19" s="43"/>
+      <c r="AP19" s="43"/>
+      <c r="AQ19" s="43"/>
+      <c r="AR19" s="43"/>
+      <c r="AS19" s="43"/>
       <c r="AT19" s="43"/>
-      <c r="AU19" s="43"/>
+      <c r="AU19" s="107"/>
       <c r="AV19" s="43"/>
       <c r="AW19" s="43"/>
       <c r="AX19" s="43"/>
       <c r="AY19" s="43"/>
       <c r="AZ19" s="43"/>
     </row>
-    <row r="20" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="95">
-        <f>SUM(B12:B19)</f>
-        <v>100</v>
-      </c>
-      <c r="C20" s="95">
-        <f>SUM(C12:C19)</f>
-        <v>59</v>
-      </c>
-      <c r="D20" s="96"/>
-      <c r="E20" s="96"/>
-      <c r="F20" s="96"/>
-      <c r="G20" s="96"/>
-      <c r="H20" s="96"/>
-      <c r="I20" s="96"/>
-      <c r="J20" s="96"/>
-      <c r="K20" s="96"/>
-      <c r="L20" s="96"/>
-      <c r="M20" s="96"/>
-      <c r="N20" s="96"/>
-      <c r="O20" s="96"/>
-      <c r="P20" s="96"/>
-      <c r="Q20" s="96"/>
-      <c r="R20" s="96"/>
-      <c r="S20" s="96"/>
-      <c r="T20" s="96"/>
-      <c r="U20" s="96"/>
-      <c r="V20" s="96"/>
-      <c r="W20" s="96"/>
-      <c r="X20" s="96"/>
-      <c r="Y20" s="96"/>
-      <c r="Z20" s="96"/>
-      <c r="AA20" s="96"/>
-      <c r="AB20" s="96"/>
-      <c r="AC20" s="96"/>
-      <c r="AD20" s="96"/>
-      <c r="AE20" s="96"/>
-      <c r="AF20" s="96"/>
-      <c r="AG20" s="96"/>
-      <c r="AH20" s="96"/>
-      <c r="AI20" s="96"/>
-      <c r="AJ20" s="96"/>
-      <c r="AK20" s="96"/>
-      <c r="AL20" s="96"/>
-      <c r="AM20" s="96"/>
-      <c r="AN20" s="96"/>
-      <c r="AO20" s="96"/>
-      <c r="AP20" s="96"/>
-      <c r="AQ20" s="96"/>
-      <c r="AR20" s="96"/>
-      <c r="AS20" s="108"/>
+    <row r="20" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A20" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="69">
+        <v>2</v>
+      </c>
+      <c r="C20" s="69">
+        <v>3</v>
+      </c>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="51"/>
+      <c r="Q20" s="51"/>
+      <c r="R20" s="51"/>
+      <c r="S20" s="51"/>
+      <c r="T20" s="51"/>
+      <c r="U20" s="51"/>
+      <c r="V20" s="51"/>
+      <c r="W20" s="51"/>
+      <c r="X20" s="51"/>
+      <c r="Y20" s="51"/>
+      <c r="Z20" s="51"/>
+      <c r="AA20" s="51"/>
+      <c r="AB20" s="51"/>
+      <c r="AC20" s="51"/>
+      <c r="AD20" s="51"/>
+      <c r="AE20" s="51"/>
+      <c r="AK20" s="43"/>
+      <c r="AL20" s="43"/>
+      <c r="AM20" s="43"/>
+      <c r="AN20" s="104"/>
+      <c r="AO20" s="43"/>
+      <c r="AP20" s="43"/>
+      <c r="AQ20" s="43"/>
+      <c r="AR20" s="43"/>
+      <c r="AS20" s="43"/>
       <c r="AT20" s="43"/>
-      <c r="AU20" s="43"/>
+      <c r="AU20" s="107"/>
       <c r="AV20" s="43"/>
       <c r="AW20" s="43"/>
       <c r="AX20" s="43"/>
@@ -2929,99 +2938,116 @@
       <c r="AZ20" s="43"/>
     </row>
     <row r="21" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A21" s="98" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="88"/>
-      <c r="C21" s="88"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="60"/>
-      <c r="I21" s="60"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="60"/>
-      <c r="L21" s="60"/>
-      <c r="M21" s="60"/>
-      <c r="N21" s="60"/>
-      <c r="O21" s="60"/>
-      <c r="P21" s="60"/>
-      <c r="Q21" s="60"/>
-      <c r="R21" s="60"/>
-      <c r="S21" s="60"/>
-      <c r="T21" s="60"/>
-      <c r="U21" s="60"/>
-      <c r="V21" s="60"/>
-      <c r="W21" s="60"/>
-      <c r="X21" s="60"/>
-      <c r="Y21" s="60"/>
-      <c r="Z21" s="60"/>
-      <c r="AA21" s="60"/>
-      <c r="AB21" s="60"/>
-      <c r="AC21" s="60"/>
-      <c r="AD21" s="60"/>
-      <c r="AE21" s="60"/>
+      <c r="A21" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="69">
+        <v>20</v>
+      </c>
+      <c r="C21" s="69">
+        <v>6</v>
+      </c>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="51"/>
+      <c r="O21" s="51"/>
+      <c r="P21" s="51"/>
+      <c r="Q21" s="51"/>
+      <c r="R21" s="51"/>
+      <c r="S21" s="51"/>
+      <c r="T21" s="51"/>
+      <c r="U21" s="51"/>
+      <c r="V21" s="51"/>
+      <c r="W21" s="51"/>
+      <c r="X21" s="51"/>
+      <c r="Y21" s="51"/>
+      <c r="Z21" s="51"/>
+      <c r="AA21" s="51"/>
+      <c r="AB21" s="51"/>
+      <c r="AC21" s="51"/>
+      <c r="AD21" s="51"/>
+      <c r="AE21" s="51"/>
+      <c r="AK21" s="43"/>
+      <c r="AL21" s="43"/>
+      <c r="AM21" s="43"/>
       <c r="AN21" s="43"/>
-      <c r="AO21" s="43"/>
-      <c r="AP21" s="43"/>
-      <c r="AQ21" s="43"/>
-      <c r="AR21" s="43"/>
-      <c r="AS21" s="107"/>
-      <c r="AT21" s="43"/>
-      <c r="AU21" s="43"/>
+      <c r="AO21" s="104"/>
+      <c r="AP21" s="104"/>
+      <c r="AQ21" s="4"/>
+      <c r="AR21" s="4"/>
+      <c r="AS21" s="4"/>
+      <c r="AT21" s="4"/>
+      <c r="AU21" s="109"/>
       <c r="AV21" s="43"/>
       <c r="AW21" s="43"/>
       <c r="AX21" s="43"/>
       <c r="AY21" s="43"/>
       <c r="AZ21" s="43"/>
     </row>
-    <row r="22" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A22" s="92" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="69">
-        <v>5</v>
-      </c>
-      <c r="C22" s="69">
-        <v>3</v>
-      </c>
-      <c r="D22" s="51"/>
-      <c r="E22" s="102"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="59"/>
-      <c r="H22" s="51"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="51"/>
-      <c r="L22" s="51"/>
-      <c r="M22" s="51"/>
-      <c r="N22" s="51"/>
-      <c r="O22" s="51"/>
-      <c r="P22" s="51"/>
-      <c r="Q22" s="51"/>
-      <c r="R22" s="51"/>
-      <c r="S22" s="51"/>
-      <c r="T22" s="51"/>
-      <c r="U22" s="51"/>
-      <c r="V22" s="51"/>
-      <c r="W22" s="51"/>
-      <c r="X22" s="51"/>
-      <c r="Y22" s="51"/>
-      <c r="Z22" s="51"/>
-      <c r="AA22" s="51"/>
-      <c r="AB22" s="51"/>
-      <c r="AC22" s="51"/>
-      <c r="AD22" s="51"/>
-      <c r="AE22" s="51"/>
-      <c r="AN22" s="43"/>
-      <c r="AO22" s="43"/>
-      <c r="AP22" s="43"/>
-      <c r="AQ22" s="43"/>
-      <c r="AR22" s="43"/>
-      <c r="AS22" s="107"/>
-      <c r="AT22" s="43"/>
-      <c r="AU22" s="43"/>
+    <row r="22" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="95">
+        <f>SUM(B13:B21)</f>
+        <v>107</v>
+      </c>
+      <c r="C22" s="95">
+        <f>SUM(C13:C21)</f>
+        <v>73</v>
+      </c>
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="96"/>
+      <c r="G22" s="96"/>
+      <c r="H22" s="96"/>
+      <c r="I22" s="96"/>
+      <c r="J22" s="96"/>
+      <c r="K22" s="96"/>
+      <c r="L22" s="96"/>
+      <c r="M22" s="96"/>
+      <c r="N22" s="96"/>
+      <c r="O22" s="96"/>
+      <c r="P22" s="96"/>
+      <c r="Q22" s="96"/>
+      <c r="R22" s="96"/>
+      <c r="S22" s="96"/>
+      <c r="T22" s="96"/>
+      <c r="U22" s="96"/>
+      <c r="V22" s="96"/>
+      <c r="W22" s="96"/>
+      <c r="X22" s="96"/>
+      <c r="Y22" s="96"/>
+      <c r="Z22" s="96"/>
+      <c r="AA22" s="96"/>
+      <c r="AB22" s="96"/>
+      <c r="AC22" s="96"/>
+      <c r="AD22" s="96"/>
+      <c r="AE22" s="96"/>
+      <c r="AF22" s="96"/>
+      <c r="AG22" s="96"/>
+      <c r="AH22" s="96"/>
+      <c r="AI22" s="96"/>
+      <c r="AJ22" s="96"/>
+      <c r="AK22" s="96"/>
+      <c r="AL22" s="96"/>
+      <c r="AM22" s="96"/>
+      <c r="AN22" s="96"/>
+      <c r="AO22" s="96"/>
+      <c r="AP22" s="96"/>
+      <c r="AQ22" s="96"/>
+      <c r="AR22" s="96"/>
+      <c r="AS22" s="96"/>
+      <c r="AT22" s="96"/>
+      <c r="AU22" s="108"/>
       <c r="AV22" s="43"/>
       <c r="AW22" s="43"/>
       <c r="AX22" s="43"/>
@@ -3029,51 +3055,47 @@
       <c r="AZ22" s="43"/>
     </row>
     <row r="23" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A23" s="92" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="69">
-        <v>2</v>
-      </c>
-      <c r="C23" s="69">
-        <v>2</v>
-      </c>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="93"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="51"/>
-      <c r="M23" s="51"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="51"/>
-      <c r="P23" s="51"/>
-      <c r="Q23" s="51"/>
-      <c r="R23" s="51"/>
-      <c r="S23" s="51"/>
-      <c r="T23" s="51"/>
-      <c r="U23" s="51"/>
-      <c r="V23" s="51"/>
-      <c r="W23" s="51"/>
-      <c r="X23" s="51"/>
-      <c r="Y23" s="51"/>
-      <c r="Z23" s="51"/>
-      <c r="AA23" s="51"/>
-      <c r="AB23" s="51"/>
-      <c r="AC23" s="51"/>
-      <c r="AD23" s="51"/>
-      <c r="AE23" s="51"/>
+      <c r="A23" s="98" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="88"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="60"/>
+      <c r="M23" s="60"/>
+      <c r="N23" s="60"/>
+      <c r="O23" s="60"/>
+      <c r="P23" s="60"/>
+      <c r="Q23" s="60"/>
+      <c r="R23" s="60"/>
+      <c r="S23" s="60"/>
+      <c r="T23" s="60"/>
+      <c r="U23" s="60"/>
+      <c r="V23" s="60"/>
+      <c r="W23" s="60"/>
+      <c r="X23" s="60"/>
+      <c r="Y23" s="60"/>
+      <c r="Z23" s="60"/>
+      <c r="AA23" s="60"/>
+      <c r="AB23" s="60"/>
+      <c r="AC23" s="60"/>
+      <c r="AD23" s="60"/>
+      <c r="AE23" s="60"/>
       <c r="AN23" s="43"/>
       <c r="AO23" s="43"/>
       <c r="AP23" s="43"/>
       <c r="AQ23" s="43"/>
       <c r="AR23" s="43"/>
-      <c r="AS23" s="107"/>
+      <c r="AS23" s="43"/>
       <c r="AT23" s="43"/>
-      <c r="AU23" s="43"/>
+      <c r="AU23" s="107"/>
       <c r="AV23" s="43"/>
       <c r="AW23" s="43"/>
       <c r="AX23" s="43"/>
@@ -3082,19 +3104,20 @@
     </row>
     <row r="24" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A24" s="92" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B24" s="69">
+        <v>5</v>
+      </c>
+      <c r="C24" s="69">
         <v>3</v>
       </c>
-      <c r="C24" s="69">
-        <v>1</v>
-      </c>
       <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="93"/>
-      <c r="H24" s="43"/>
+      <c r="E24" s="102"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="51"/>
       <c r="J24" s="51"/>
       <c r="K24" s="51"/>
       <c r="L24" s="51"/>
@@ -3122,9 +3145,9 @@
       <c r="AP24" s="43"/>
       <c r="AQ24" s="43"/>
       <c r="AR24" s="43"/>
-      <c r="AS24" s="107"/>
+      <c r="AS24" s="43"/>
       <c r="AT24" s="43"/>
-      <c r="AU24" s="43"/>
+      <c r="AU24" s="107"/>
       <c r="AV24" s="43"/>
       <c r="AW24" s="43"/>
       <c r="AX24" s="43"/>
@@ -3133,20 +3156,20 @@
     </row>
     <row r="25" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A25" s="92" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B25" s="69">
         <v>2</v>
       </c>
       <c r="C25" s="69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" s="51"/>
       <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
+      <c r="F25" s="93"/>
       <c r="G25" s="51"/>
-      <c r="H25" s="93"/>
-      <c r="I25" s="43"/>
+      <c r="H25" s="51"/>
+      <c r="I25" s="51"/>
       <c r="J25" s="51"/>
       <c r="K25" s="51"/>
       <c r="L25" s="51"/>
@@ -3174,9 +3197,9 @@
       <c r="AP25" s="43"/>
       <c r="AQ25" s="43"/>
       <c r="AR25" s="43"/>
-      <c r="AS25" s="107"/>
+      <c r="AS25" s="43"/>
       <c r="AT25" s="43"/>
-      <c r="AU25" s="43"/>
+      <c r="AU25" s="107"/>
       <c r="AV25" s="43"/>
       <c r="AW25" s="43"/>
       <c r="AX25" s="43"/>
@@ -3185,23 +3208,22 @@
     </row>
     <row r="26" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A26" s="92" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="B26" s="69">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C26" s="69">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D26" s="51"/>
       <c r="E26" s="51"/>
       <c r="F26" s="51"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="51"/>
-      <c r="I26" s="93"/>
-      <c r="J26" s="93"/>
-      <c r="K26" s="93"/>
-      <c r="L26" s="93"/>
+      <c r="G26" s="93"/>
+      <c r="H26" s="43"/>
+      <c r="J26" s="51"/>
+      <c r="K26" s="51"/>
+      <c r="L26" s="51"/>
       <c r="M26" s="51"/>
       <c r="N26" s="51"/>
       <c r="O26" s="51"/>
@@ -3226,9 +3248,9 @@
       <c r="AP26" s="43"/>
       <c r="AQ26" s="43"/>
       <c r="AR26" s="43"/>
-      <c r="AS26" s="107"/>
+      <c r="AS26" s="43"/>
       <c r="AT26" s="43"/>
-      <c r="AU26" s="43"/>
+      <c r="AU26" s="107"/>
       <c r="AV26" s="43"/>
       <c r="AW26" s="43"/>
       <c r="AX26" s="43"/>
@@ -3237,25 +3259,25 @@
     </row>
     <row r="27" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A27" s="92" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="B27" s="69">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C27" s="69">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D27" s="51"/>
       <c r="E27" s="51"/>
       <c r="F27" s="51"/>
       <c r="G27" s="51"/>
-      <c r="H27" s="51"/>
-      <c r="I27" s="51"/>
+      <c r="H27" s="93"/>
+      <c r="I27" s="43"/>
       <c r="J27" s="51"/>
-      <c r="K27" s="59"/>
+      <c r="K27" s="51"/>
       <c r="L27" s="51"/>
-      <c r="M27" s="93"/>
-      <c r="N27" s="103"/>
+      <c r="M27" s="51"/>
+      <c r="N27" s="51"/>
       <c r="O27" s="51"/>
       <c r="P27" s="51"/>
       <c r="Q27" s="51"/>
@@ -3278,9 +3300,9 @@
       <c r="AP27" s="43"/>
       <c r="AQ27" s="43"/>
       <c r="AR27" s="43"/>
-      <c r="AS27" s="107"/>
+      <c r="AS27" s="43"/>
       <c r="AT27" s="43"/>
-      <c r="AU27" s="43"/>
+      <c r="AU27" s="107"/>
       <c r="AV27" s="43"/>
       <c r="AW27" s="43"/>
       <c r="AX27" s="43"/>
@@ -3289,87 +3311,102 @@
     </row>
     <row r="28" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A28" s="92" t="s">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="B28" s="69">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C28" s="69">
-        <v>5</v>
-      </c>
-      <c r="O28" s="104"/>
-      <c r="P28" s="104"/>
-      <c r="Q28" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="93"/>
+      <c r="J28" s="93"/>
+      <c r="K28" s="93"/>
+      <c r="L28" s="93"/>
+      <c r="M28" s="51"/>
+      <c r="N28" s="51"/>
+      <c r="O28" s="51"/>
+      <c r="P28" s="51"/>
+      <c r="Q28" s="51"/>
+      <c r="R28" s="51"/>
+      <c r="S28" s="51"/>
+      <c r="T28" s="51"/>
+      <c r="U28" s="51"/>
+      <c r="V28" s="51"/>
+      <c r="W28" s="51"/>
+      <c r="X28" s="51"/>
+      <c r="Y28" s="51"/>
+      <c r="Z28" s="51"/>
+      <c r="AA28" s="51"/>
+      <c r="AB28" s="51"/>
+      <c r="AC28" s="51"/>
+      <c r="AD28" s="51"/>
+      <c r="AE28" s="51"/>
       <c r="AN28" s="43"/>
       <c r="AO28" s="43"/>
       <c r="AP28" s="43"/>
       <c r="AQ28" s="43"/>
       <c r="AR28" s="43"/>
-      <c r="AS28" s="107"/>
+      <c r="AS28" s="43"/>
       <c r="AT28" s="43"/>
-      <c r="AU28" s="43"/>
+      <c r="AU28" s="107"/>
       <c r="AV28" s="43"/>
       <c r="AW28" s="43"/>
       <c r="AX28" s="43"/>
       <c r="AY28" s="43"/>
       <c r="AZ28" s="43"/>
     </row>
-    <row r="29" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="95">
-        <f>SUM(B22:B28)</f>
-        <v>36</v>
-      </c>
-      <c r="C29" s="95">
-        <f>SUM(C22:C28)</f>
-        <v>26</v>
-      </c>
-      <c r="D29" s="96"/>
-      <c r="E29" s="96"/>
-      <c r="F29" s="96"/>
-      <c r="G29" s="96"/>
-      <c r="H29" s="96"/>
-      <c r="I29" s="96"/>
-      <c r="J29" s="96"/>
-      <c r="K29" s="96"/>
-      <c r="L29" s="96"/>
-      <c r="M29" s="96"/>
-      <c r="N29" s="96"/>
-      <c r="O29" s="96"/>
-      <c r="P29" s="96"/>
-      <c r="Q29" s="96"/>
-      <c r="R29" s="96"/>
-      <c r="S29" s="96"/>
-      <c r="T29" s="96"/>
-      <c r="U29" s="96"/>
-      <c r="V29" s="96"/>
-      <c r="W29" s="96"/>
-      <c r="X29" s="96"/>
-      <c r="Y29" s="96"/>
-      <c r="Z29" s="96"/>
-      <c r="AA29" s="96"/>
-      <c r="AB29" s="96"/>
-      <c r="AC29" s="96"/>
-      <c r="AD29" s="96"/>
-      <c r="AE29" s="96"/>
-      <c r="AF29" s="96"/>
-      <c r="AG29" s="96"/>
-      <c r="AH29" s="96"/>
-      <c r="AI29" s="96"/>
-      <c r="AJ29" s="96"/>
-      <c r="AK29" s="96"/>
-      <c r="AL29" s="96"/>
-      <c r="AM29" s="96"/>
-      <c r="AN29" s="96"/>
-      <c r="AO29" s="96"/>
-      <c r="AP29" s="96"/>
-      <c r="AQ29" s="96"/>
-      <c r="AR29" s="96"/>
-      <c r="AS29" s="108"/>
+    <row r="29" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A29" s="92" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="69">
+        <v>6</v>
+      </c>
+      <c r="C29" s="69">
+        <v>5</v>
+      </c>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="59"/>
+      <c r="L29" s="51"/>
+      <c r="M29" s="93"/>
+      <c r="N29" s="93"/>
+      <c r="O29" s="103"/>
+      <c r="P29" s="51"/>
+      <c r="Q29" s="51"/>
+      <c r="R29" s="51"/>
+      <c r="S29" s="51"/>
+      <c r="T29" s="51"/>
+      <c r="U29" s="51"/>
+      <c r="V29" s="51"/>
+      <c r="W29" s="51"/>
+      <c r="X29" s="51"/>
+      <c r="Y29" s="51"/>
+      <c r="Z29" s="51"/>
+      <c r="AA29" s="51"/>
+      <c r="AB29" s="51"/>
+      <c r="AC29" s="51"/>
+      <c r="AD29" s="51"/>
+      <c r="AE29" s="51"/>
+      <c r="AN29" s="43"/>
+      <c r="AO29" s="43"/>
+      <c r="AP29" s="43"/>
+      <c r="AQ29" s="43"/>
+      <c r="AR29" s="43"/>
+      <c r="AS29" s="43"/>
       <c r="AT29" s="43"/>
-      <c r="AU29" s="43"/>
+      <c r="AU29" s="107"/>
       <c r="AV29" s="43"/>
       <c r="AW29" s="43"/>
       <c r="AX29" s="43"/>
@@ -3377,99 +3414,89 @@
       <c r="AZ29" s="43"/>
     </row>
     <row r="30" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A30" s="98" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="88"/>
-      <c r="C30" s="88"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="60"/>
-      <c r="K30" s="60"/>
-      <c r="L30" s="60"/>
-      <c r="M30" s="60"/>
-      <c r="N30" s="60"/>
-      <c r="O30" s="60"/>
-      <c r="P30" s="60"/>
-      <c r="Q30" s="60"/>
-      <c r="R30" s="60"/>
-      <c r="S30" s="60"/>
-      <c r="T30" s="60"/>
-      <c r="U30" s="60"/>
-      <c r="V30" s="60"/>
-      <c r="W30" s="60"/>
-      <c r="X30" s="60"/>
-      <c r="Y30" s="60"/>
-      <c r="Z30" s="60"/>
-      <c r="AA30" s="60"/>
-      <c r="AB30" s="60"/>
-      <c r="AC30" s="60"/>
-      <c r="AD30" s="60"/>
-      <c r="AE30" s="60"/>
+      <c r="A30" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="69">
+        <v>3</v>
+      </c>
+      <c r="C30" s="69">
+        <v>7</v>
+      </c>
+      <c r="O30" s="43"/>
+      <c r="P30" s="104"/>
+      <c r="Q30" s="104"/>
+      <c r="R30" s="104"/>
       <c r="AN30" s="43"/>
       <c r="AO30" s="43"/>
       <c r="AP30" s="43"/>
       <c r="AQ30" s="43"/>
       <c r="AR30" s="43"/>
-      <c r="AS30" s="107"/>
+      <c r="AS30" s="43"/>
       <c r="AT30" s="43"/>
-      <c r="AU30" s="43"/>
+      <c r="AU30" s="107"/>
       <c r="AV30" s="43"/>
       <c r="AW30" s="43"/>
       <c r="AX30" s="43"/>
       <c r="AY30" s="43"/>
       <c r="AZ30" s="43"/>
     </row>
-    <row r="31" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A31" s="92" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="69">
-        <v>6</v>
-      </c>
-      <c r="C31" s="69">
-        <v>12</v>
-      </c>
-      <c r="D31" s="51"/>
-      <c r="E31" s="93"/>
-      <c r="F31" s="93"/>
-      <c r="G31" s="93"/>
-      <c r="H31" s="103"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
-      <c r="K31" s="51"/>
-      <c r="L31" s="51"/>
-      <c r="M31" s="51"/>
-      <c r="N31" s="51"/>
-      <c r="O31" s="51"/>
-      <c r="P31" s="51"/>
-      <c r="Q31" s="51"/>
-      <c r="R31" s="51"/>
-      <c r="S31" s="51"/>
-      <c r="T31" s="51"/>
-      <c r="U31" s="51"/>
-      <c r="V31" s="51"/>
-      <c r="W31" s="51"/>
-      <c r="X31" s="51"/>
-      <c r="Y31" s="51"/>
-      <c r="Z31" s="51"/>
-      <c r="AA31" s="51"/>
-      <c r="AB31" s="51"/>
-      <c r="AC31" s="51"/>
-      <c r="AD31" s="51"/>
-      <c r="AE31" s="51"/>
-      <c r="AN31" s="43"/>
-      <c r="AO31" s="43"/>
-      <c r="AP31" s="43"/>
-      <c r="AQ31" s="43"/>
-      <c r="AR31" s="43"/>
-      <c r="AS31" s="107"/>
-      <c r="AT31" s="43"/>
-      <c r="AU31" s="43"/>
+    <row r="31" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="95">
+        <f>SUM(B24:B30)</f>
+        <v>36</v>
+      </c>
+      <c r="C31" s="95">
+        <f>SUM(C24:C30)</f>
+        <v>32</v>
+      </c>
+      <c r="D31" s="96"/>
+      <c r="E31" s="96"/>
+      <c r="F31" s="96"/>
+      <c r="G31" s="96"/>
+      <c r="H31" s="96"/>
+      <c r="I31" s="96"/>
+      <c r="J31" s="96"/>
+      <c r="K31" s="96"/>
+      <c r="L31" s="96"/>
+      <c r="M31" s="96"/>
+      <c r="N31" s="96"/>
+      <c r="O31" s="96"/>
+      <c r="P31" s="96"/>
+      <c r="Q31" s="96"/>
+      <c r="R31" s="96"/>
+      <c r="S31" s="96"/>
+      <c r="T31" s="96"/>
+      <c r="U31" s="96"/>
+      <c r="V31" s="96"/>
+      <c r="W31" s="96"/>
+      <c r="X31" s="96"/>
+      <c r="Y31" s="96"/>
+      <c r="Z31" s="96"/>
+      <c r="AA31" s="96"/>
+      <c r="AB31" s="96"/>
+      <c r="AC31" s="96"/>
+      <c r="AD31" s="96"/>
+      <c r="AE31" s="96"/>
+      <c r="AF31" s="96"/>
+      <c r="AG31" s="96"/>
+      <c r="AH31" s="96"/>
+      <c r="AI31" s="96"/>
+      <c r="AJ31" s="96"/>
+      <c r="AK31" s="96"/>
+      <c r="AL31" s="96"/>
+      <c r="AM31" s="96"/>
+      <c r="AN31" s="96"/>
+      <c r="AO31" s="96"/>
+      <c r="AP31" s="96"/>
+      <c r="AQ31" s="96"/>
+      <c r="AR31" s="96"/>
+      <c r="AS31" s="96"/>
+      <c r="AT31" s="96"/>
+      <c r="AU31" s="108"/>
       <c r="AV31" s="43"/>
       <c r="AW31" s="43"/>
       <c r="AX31" s="43"/>
@@ -3477,51 +3504,47 @@
       <c r="AZ31" s="43"/>
     </row>
     <row r="32" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A32" s="92" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="69">
-        <v>4</v>
-      </c>
-      <c r="C32" s="69">
-        <v>5</v>
-      </c>
-      <c r="D32" s="51"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="51"/>
-      <c r="G32" s="51"/>
-      <c r="H32" s="51"/>
-      <c r="I32" s="93"/>
-      <c r="J32" s="93"/>
-      <c r="K32" s="51"/>
-      <c r="L32" s="51"/>
-      <c r="M32" s="51"/>
-      <c r="N32" s="51"/>
-      <c r="O32" s="51"/>
-      <c r="P32" s="51"/>
-      <c r="Q32" s="51"/>
-      <c r="R32" s="51"/>
-      <c r="S32" s="51"/>
-      <c r="T32" s="51"/>
-      <c r="U32" s="51"/>
-      <c r="V32" s="51"/>
-      <c r="W32" s="51"/>
-      <c r="X32" s="51"/>
-      <c r="Y32" s="51"/>
-      <c r="Z32" s="51"/>
-      <c r="AA32" s="51"/>
-      <c r="AB32" s="51"/>
-      <c r="AC32" s="51"/>
-      <c r="AD32" s="51"/>
-      <c r="AE32" s="51"/>
+      <c r="A32" s="98" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="88"/>
+      <c r="C32" s="88"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="60"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="60"/>
+      <c r="K32" s="60"/>
+      <c r="L32" s="60"/>
+      <c r="M32" s="60"/>
+      <c r="N32" s="60"/>
+      <c r="O32" s="60"/>
+      <c r="P32" s="60"/>
+      <c r="Q32" s="60"/>
+      <c r="R32" s="60"/>
+      <c r="S32" s="60"/>
+      <c r="T32" s="60"/>
+      <c r="U32" s="60"/>
+      <c r="V32" s="60"/>
+      <c r="W32" s="60"/>
+      <c r="X32" s="60"/>
+      <c r="Y32" s="60"/>
+      <c r="Z32" s="60"/>
+      <c r="AA32" s="60"/>
+      <c r="AB32" s="60"/>
+      <c r="AC32" s="60"/>
+      <c r="AD32" s="60"/>
+      <c r="AE32" s="60"/>
       <c r="AN32" s="43"/>
       <c r="AO32" s="43"/>
       <c r="AP32" s="43"/>
       <c r="AQ32" s="43"/>
       <c r="AR32" s="43"/>
-      <c r="AS32" s="107"/>
+      <c r="AS32" s="43"/>
       <c r="AT32" s="43"/>
-      <c r="AU32" s="43"/>
+      <c r="AU32" s="107"/>
       <c r="AV32" s="43"/>
       <c r="AW32" s="43"/>
       <c r="AX32" s="43"/>
@@ -3530,22 +3553,22 @@
     </row>
     <row r="33" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A33" s="92" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B33" s="69">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C33" s="69">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="51"/>
+      <c r="E33" s="93"/>
+      <c r="F33" s="93"/>
+      <c r="G33" s="93"/>
+      <c r="H33" s="93"/>
       <c r="I33" s="51"/>
       <c r="J33" s="51"/>
-      <c r="K33" s="94"/>
+      <c r="K33" s="51"/>
       <c r="L33" s="51"/>
       <c r="M33" s="51"/>
       <c r="N33" s="51"/>
@@ -3571,9 +3594,9 @@
       <c r="AP33" s="43"/>
       <c r="AQ33" s="43"/>
       <c r="AR33" s="43"/>
-      <c r="AS33" s="107"/>
+      <c r="AS33" s="43"/>
       <c r="AT33" s="43"/>
-      <c r="AU33" s="43"/>
+      <c r="AU33" s="107"/>
       <c r="AV33" s="43"/>
       <c r="AW33" s="43"/>
       <c r="AX33" s="43"/>
@@ -3582,7 +3605,7 @@
     </row>
     <row r="34" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A34" s="92" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="B34" s="69">
         <v>4</v>
@@ -3595,11 +3618,11 @@
       <c r="F34" s="51"/>
       <c r="G34" s="51"/>
       <c r="H34" s="51"/>
-      <c r="I34" s="51"/>
-      <c r="J34" s="51"/>
+      <c r="I34" s="93"/>
+      <c r="J34" s="93"/>
       <c r="K34" s="51"/>
-      <c r="L34" s="93"/>
-      <c r="M34" s="94"/>
+      <c r="L34" s="51"/>
+      <c r="M34" s="51"/>
       <c r="N34" s="51"/>
       <c r="O34" s="51"/>
       <c r="P34" s="51"/>
@@ -3623,9 +3646,9 @@
       <c r="AP34" s="43"/>
       <c r="AQ34" s="43"/>
       <c r="AR34" s="43"/>
-      <c r="AS34" s="107"/>
+      <c r="AS34" s="43"/>
       <c r="AT34" s="43"/>
-      <c r="AU34" s="43"/>
+      <c r="AU34" s="107"/>
       <c r="AV34" s="43"/>
       <c r="AW34" s="43"/>
       <c r="AX34" s="43"/>
@@ -3634,13 +3657,13 @@
     </row>
     <row r="35" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A35" s="92" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="B35" s="69">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" s="69">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D35" s="51"/>
       <c r="E35" s="51"/>
@@ -3649,11 +3672,11 @@
       <c r="H35" s="51"/>
       <c r="I35" s="51"/>
       <c r="J35" s="51"/>
-      <c r="K35" s="51"/>
+      <c r="K35" s="94"/>
       <c r="L35" s="51"/>
       <c r="M35" s="51"/>
-      <c r="N35" s="93"/>
-      <c r="O35" s="94"/>
+      <c r="N35" s="51"/>
+      <c r="O35" s="51"/>
       <c r="P35" s="51"/>
       <c r="Q35" s="51"/>
       <c r="R35" s="51"/>
@@ -3675,9 +3698,9 @@
       <c r="AP35" s="43"/>
       <c r="AQ35" s="43"/>
       <c r="AR35" s="43"/>
-      <c r="AS35" s="107"/>
+      <c r="AS35" s="43"/>
       <c r="AT35" s="43"/>
-      <c r="AU35" s="43"/>
+      <c r="AU35" s="107"/>
       <c r="AV35" s="43"/>
       <c r="AW35" s="43"/>
       <c r="AX35" s="43"/>
@@ -3686,10 +3709,10 @@
     </row>
     <row r="36" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A36" s="92" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B36" s="69">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C36" s="69">
         <v>6</v>
@@ -3702,14 +3725,14 @@
       <c r="I36" s="51"/>
       <c r="J36" s="51"/>
       <c r="K36" s="51"/>
-      <c r="L36" s="51"/>
-      <c r="M36" s="51"/>
+      <c r="L36" s="93"/>
+      <c r="M36" s="93"/>
       <c r="N36" s="51"/>
       <c r="O36" s="51"/>
-      <c r="P36" s="93"/>
-      <c r="Q36" s="93"/>
-      <c r="R36" s="103"/>
-      <c r="S36" s="94"/>
+      <c r="P36" s="51"/>
+      <c r="Q36" s="51"/>
+      <c r="R36" s="51"/>
+      <c r="S36" s="51"/>
       <c r="T36" s="51"/>
       <c r="U36" s="51"/>
       <c r="V36" s="51"/>
@@ -3727,9 +3750,9 @@
       <c r="AP36" s="43"/>
       <c r="AQ36" s="43"/>
       <c r="AR36" s="43"/>
-      <c r="AS36" s="107"/>
+      <c r="AS36" s="43"/>
       <c r="AT36" s="43"/>
-      <c r="AU36" s="43"/>
+      <c r="AU36" s="107"/>
       <c r="AV36" s="43"/>
       <c r="AW36" s="43"/>
       <c r="AX36" s="43"/>
@@ -3738,13 +3761,13 @@
     </row>
     <row r="37" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A37" s="92" t="s">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="B37" s="69">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C37" s="69">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D37" s="51"/>
       <c r="E37" s="51"/>
@@ -3756,15 +3779,15 @@
       <c r="K37" s="51"/>
       <c r="L37" s="51"/>
       <c r="M37" s="51"/>
-      <c r="N37" s="51"/>
-      <c r="O37" s="51"/>
+      <c r="N37" s="93"/>
+      <c r="O37" s="93"/>
       <c r="P37" s="51"/>
       <c r="Q37" s="51"/>
       <c r="R37" s="51"/>
       <c r="S37" s="51"/>
-      <c r="T37" s="93"/>
-      <c r="U37" s="93"/>
-      <c r="V37" s="94"/>
+      <c r="T37" s="51"/>
+      <c r="U37" s="51"/>
+      <c r="V37" s="51"/>
       <c r="W37" s="51"/>
       <c r="X37" s="51"/>
       <c r="Y37" s="51"/>
@@ -3774,77 +3797,66 @@
       <c r="AC37" s="51"/>
       <c r="AD37" s="51"/>
       <c r="AE37" s="51"/>
-      <c r="AF37" s="43"/>
       <c r="AN37" s="43"/>
       <c r="AO37" s="43"/>
       <c r="AP37" s="43"/>
       <c r="AQ37" s="43"/>
       <c r="AR37" s="43"/>
-      <c r="AS37" s="107"/>
+      <c r="AS37" s="43"/>
       <c r="AT37" s="43"/>
-      <c r="AU37" s="43"/>
+      <c r="AU37" s="107"/>
       <c r="AV37" s="43"/>
       <c r="AW37" s="43"/>
       <c r="AX37" s="43"/>
       <c r="AY37" s="43"/>
       <c r="AZ37" s="43"/>
     </row>
-    <row r="38" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" s="95">
-        <f>SUM(B31:B37)</f>
-        <v>35</v>
-      </c>
-      <c r="C38" s="95">
-        <f>SUM(C31:C37)</f>
-        <v>38</v>
-      </c>
-      <c r="D38" s="96"/>
-      <c r="E38" s="96"/>
-      <c r="F38" s="96"/>
-      <c r="G38" s="96"/>
-      <c r="H38" s="96"/>
-      <c r="I38" s="96"/>
-      <c r="J38" s="96"/>
-      <c r="K38" s="96"/>
-      <c r="L38" s="96"/>
-      <c r="M38" s="96"/>
-      <c r="N38" s="96"/>
-      <c r="O38" s="96"/>
-      <c r="P38" s="96"/>
-      <c r="Q38" s="96"/>
-      <c r="R38" s="96"/>
-      <c r="S38" s="96"/>
-      <c r="T38" s="96"/>
-      <c r="U38" s="96"/>
-      <c r="V38" s="96"/>
-      <c r="W38" s="96"/>
-      <c r="X38" s="96"/>
-      <c r="Y38" s="96"/>
-      <c r="Z38" s="96"/>
-      <c r="AA38" s="96"/>
-      <c r="AB38" s="96"/>
-      <c r="AC38" s="96"/>
-      <c r="AD38" s="96"/>
-      <c r="AE38" s="96"/>
-      <c r="AF38" s="96"/>
-      <c r="AG38" s="96"/>
-      <c r="AH38" s="96"/>
-      <c r="AI38" s="96"/>
-      <c r="AJ38" s="96"/>
-      <c r="AK38" s="96"/>
-      <c r="AL38" s="96"/>
-      <c r="AM38" s="96"/>
-      <c r="AN38" s="96"/>
-      <c r="AO38" s="96"/>
-      <c r="AP38" s="96"/>
-      <c r="AQ38" s="96"/>
-      <c r="AR38" s="96"/>
-      <c r="AS38" s="108"/>
+    <row r="38" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A38" s="92" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="69">
+        <v>10</v>
+      </c>
+      <c r="C38" s="69">
+        <v>7</v>
+      </c>
+      <c r="D38" s="51"/>
+      <c r="E38" s="51"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="51"/>
+      <c r="I38" s="51"/>
+      <c r="J38" s="51"/>
+      <c r="K38" s="51"/>
+      <c r="L38" s="51"/>
+      <c r="M38" s="51"/>
+      <c r="N38" s="51"/>
+      <c r="O38" s="51"/>
+      <c r="P38" s="93"/>
+      <c r="Q38" s="93"/>
+      <c r="R38" s="93"/>
+      <c r="S38" s="94"/>
+      <c r="T38" s="51"/>
+      <c r="U38" s="51"/>
+      <c r="V38" s="51"/>
+      <c r="W38" s="51"/>
+      <c r="X38" s="51"/>
+      <c r="Y38" s="51"/>
+      <c r="Z38" s="51"/>
+      <c r="AA38" s="51"/>
+      <c r="AB38" s="51"/>
+      <c r="AC38" s="51"/>
+      <c r="AD38" s="51"/>
+      <c r="AE38" s="51"/>
+      <c r="AN38" s="43"/>
+      <c r="AO38" s="43"/>
+      <c r="AP38" s="43"/>
+      <c r="AQ38" s="43"/>
+      <c r="AR38" s="43"/>
+      <c r="AS38" s="43"/>
       <c r="AT38" s="43"/>
-      <c r="AU38" s="43"/>
+      <c r="AU38" s="107"/>
       <c r="AV38" s="43"/>
       <c r="AW38" s="43"/>
       <c r="AX38" s="43"/>
@@ -3852,99 +3864,114 @@
       <c r="AZ38" s="43"/>
     </row>
     <row r="39" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A39" s="98" t="s">
-        <v>31</v>
-      </c>
-      <c r="B39" s="88"/>
-      <c r="C39" s="88"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="60"/>
-      <c r="F39" s="60"/>
-      <c r="G39" s="60"/>
-      <c r="H39" s="60"/>
-      <c r="I39" s="60"/>
-      <c r="J39" s="60"/>
-      <c r="K39" s="60"/>
-      <c r="L39" s="60"/>
-      <c r="M39" s="60"/>
-      <c r="N39" s="60"/>
-      <c r="O39" s="60"/>
-      <c r="P39" s="60"/>
-      <c r="Q39" s="60"/>
-      <c r="R39" s="60"/>
-      <c r="S39" s="60"/>
-      <c r="T39" s="60"/>
-      <c r="U39" s="60"/>
-      <c r="V39" s="60"/>
-      <c r="W39" s="60"/>
-      <c r="X39" s="60"/>
-      <c r="Y39" s="60"/>
-      <c r="Z39" s="60"/>
-      <c r="AA39" s="60"/>
-      <c r="AB39" s="60"/>
-      <c r="AC39" s="60"/>
-      <c r="AD39" s="60"/>
-      <c r="AE39" s="60"/>
+      <c r="A39" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="69">
+        <v>6</v>
+      </c>
+      <c r="C39" s="69">
+        <v>6</v>
+      </c>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="51"/>
+      <c r="N39" s="51"/>
+      <c r="O39" s="51"/>
+      <c r="P39" s="51"/>
+      <c r="Q39" s="51"/>
+      <c r="R39" s="51"/>
+      <c r="S39" s="51"/>
+      <c r="T39" s="93"/>
+      <c r="U39" s="93"/>
+      <c r="V39" s="94"/>
+      <c r="W39" s="51"/>
+      <c r="X39" s="51"/>
+      <c r="Y39" s="51"/>
+      <c r="Z39" s="51"/>
+      <c r="AA39" s="51"/>
+      <c r="AB39" s="51"/>
+      <c r="AC39" s="51"/>
+      <c r="AD39" s="51"/>
+      <c r="AE39" s="51"/>
+      <c r="AF39" s="43"/>
       <c r="AN39" s="43"/>
       <c r="AO39" s="43"/>
       <c r="AP39" s="43"/>
       <c r="AQ39" s="43"/>
       <c r="AR39" s="43"/>
-      <c r="AS39" s="107"/>
+      <c r="AS39" s="43"/>
       <c r="AT39" s="43"/>
-      <c r="AU39" s="43"/>
+      <c r="AU39" s="107"/>
       <c r="AV39" s="43"/>
       <c r="AW39" s="43"/>
       <c r="AX39" s="43"/>
       <c r="AY39" s="43"/>
       <c r="AZ39" s="43"/>
     </row>
-    <row r="40" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A40" s="92" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="69">
+    <row r="40" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="69">
-        <v>3</v>
-      </c>
-      <c r="D40" s="51"/>
-      <c r="E40" s="93"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="51"/>
-      <c r="I40" s="51"/>
-      <c r="J40" s="51"/>
-      <c r="K40" s="51"/>
-      <c r="L40" s="51"/>
-      <c r="M40" s="51"/>
-      <c r="N40" s="51"/>
-      <c r="O40" s="51"/>
-      <c r="P40" s="51"/>
-      <c r="Q40" s="51"/>
-      <c r="R40" s="51"/>
-      <c r="S40" s="51"/>
-      <c r="T40" s="51"/>
-      <c r="U40" s="51"/>
-      <c r="V40" s="51"/>
-      <c r="W40" s="51"/>
-      <c r="X40" s="51"/>
-      <c r="Y40" s="51"/>
-      <c r="Z40" s="51"/>
-      <c r="AA40" s="51"/>
-      <c r="AB40" s="51"/>
-      <c r="AC40" s="51"/>
-      <c r="AD40" s="51"/>
-      <c r="AE40" s="51"/>
-      <c r="AN40" s="43"/>
-      <c r="AO40" s="43"/>
-      <c r="AP40" s="43"/>
-      <c r="AQ40" s="43"/>
-      <c r="AR40" s="43"/>
-      <c r="AS40" s="107"/>
-      <c r="AT40" s="43"/>
-      <c r="AU40" s="43"/>
+      <c r="B40" s="95">
+        <f>SUM(B33:B39)</f>
+        <v>35</v>
+      </c>
+      <c r="C40" s="95">
+        <f>SUM(C33:C39)</f>
+        <v>40</v>
+      </c>
+      <c r="D40" s="96"/>
+      <c r="E40" s="96"/>
+      <c r="F40" s="96"/>
+      <c r="G40" s="96"/>
+      <c r="H40" s="96"/>
+      <c r="I40" s="96"/>
+      <c r="J40" s="96"/>
+      <c r="K40" s="96"/>
+      <c r="L40" s="96"/>
+      <c r="M40" s="96"/>
+      <c r="N40" s="96"/>
+      <c r="O40" s="96"/>
+      <c r="P40" s="96"/>
+      <c r="Q40" s="96"/>
+      <c r="R40" s="96"/>
+      <c r="S40" s="96"/>
+      <c r="T40" s="96"/>
+      <c r="U40" s="96"/>
+      <c r="V40" s="96"/>
+      <c r="W40" s="96"/>
+      <c r="X40" s="96"/>
+      <c r="Y40" s="96"/>
+      <c r="Z40" s="96"/>
+      <c r="AA40" s="96"/>
+      <c r="AB40" s="96"/>
+      <c r="AC40" s="96"/>
+      <c r="AD40" s="96"/>
+      <c r="AE40" s="96"/>
+      <c r="AF40" s="96"/>
+      <c r="AG40" s="96"/>
+      <c r="AH40" s="96"/>
+      <c r="AI40" s="96"/>
+      <c r="AJ40" s="96"/>
+      <c r="AK40" s="96"/>
+      <c r="AL40" s="96"/>
+      <c r="AM40" s="96"/>
+      <c r="AN40" s="96"/>
+      <c r="AO40" s="96"/>
+      <c r="AP40" s="96"/>
+      <c r="AQ40" s="96"/>
+      <c r="AR40" s="96"/>
+      <c r="AS40" s="96"/>
+      <c r="AT40" s="96"/>
+      <c r="AU40" s="108"/>
       <c r="AV40" s="43"/>
       <c r="AW40" s="43"/>
       <c r="AX40" s="43"/>
@@ -3952,51 +3979,47 @@
       <c r="AZ40" s="43"/>
     </row>
     <row r="41" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A41" s="92" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41" s="69">
-        <v>10</v>
-      </c>
-      <c r="C41" s="69">
-        <v>6</v>
-      </c>
-      <c r="D41" s="51"/>
-      <c r="E41" s="51"/>
-      <c r="F41" s="93"/>
-      <c r="G41" s="103"/>
-      <c r="H41" s="94"/>
-      <c r="I41" s="51"/>
-      <c r="J41" s="51"/>
-      <c r="K41" s="51"/>
-      <c r="L41" s="51"/>
-      <c r="M41" s="51"/>
-      <c r="N41" s="51"/>
-      <c r="O41" s="51"/>
-      <c r="P41" s="51"/>
-      <c r="Q41" s="51"/>
-      <c r="R41" s="51"/>
-      <c r="S41" s="51"/>
-      <c r="T41" s="51"/>
-      <c r="U41" s="51"/>
-      <c r="V41" s="51"/>
-      <c r="W41" s="51"/>
-      <c r="X41" s="51"/>
-      <c r="Y41" s="51"/>
-      <c r="Z41" s="51"/>
-      <c r="AA41" s="51"/>
-      <c r="AB41" s="51"/>
-      <c r="AC41" s="51"/>
-      <c r="AD41" s="51"/>
-      <c r="AE41" s="51"/>
+      <c r="A41" s="98" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="88"/>
+      <c r="C41" s="88"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="60"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="60"/>
+      <c r="H41" s="60"/>
+      <c r="I41" s="60"/>
+      <c r="J41" s="60"/>
+      <c r="K41" s="60"/>
+      <c r="L41" s="60"/>
+      <c r="M41" s="60"/>
+      <c r="N41" s="60"/>
+      <c r="O41" s="60"/>
+      <c r="P41" s="60"/>
+      <c r="Q41" s="60"/>
+      <c r="R41" s="60"/>
+      <c r="S41" s="60"/>
+      <c r="T41" s="60"/>
+      <c r="U41" s="60"/>
+      <c r="V41" s="60"/>
+      <c r="W41" s="60"/>
+      <c r="X41" s="60"/>
+      <c r="Y41" s="60"/>
+      <c r="Z41" s="60"/>
+      <c r="AA41" s="60"/>
+      <c r="AB41" s="60"/>
+      <c r="AC41" s="60"/>
+      <c r="AD41" s="60"/>
+      <c r="AE41" s="60"/>
       <c r="AN41" s="43"/>
       <c r="AO41" s="43"/>
       <c r="AP41" s="43"/>
       <c r="AQ41" s="43"/>
       <c r="AR41" s="43"/>
-      <c r="AS41" s="107"/>
+      <c r="AS41" s="43"/>
       <c r="AT41" s="43"/>
-      <c r="AU41" s="43"/>
+      <c r="AU41" s="107"/>
       <c r="AV41" s="43"/>
       <c r="AW41" s="43"/>
       <c r="AX41" s="43"/>
@@ -4005,26 +4028,26 @@
     </row>
     <row r="42" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A42" s="92" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B42" s="69">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C42" s="69">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D42" s="51"/>
-      <c r="E42" s="51"/>
+      <c r="E42" s="93"/>
       <c r="F42" s="51"/>
       <c r="G42" s="51"/>
       <c r="H42" s="51"/>
-      <c r="I42" s="93"/>
-      <c r="J42" s="93"/>
-      <c r="K42" s="94"/>
-      <c r="L42" s="94"/>
-      <c r="M42" s="94"/>
-      <c r="N42" s="94"/>
-      <c r="O42" s="94"/>
+      <c r="I42" s="51"/>
+      <c r="J42" s="51"/>
+      <c r="K42" s="51"/>
+      <c r="L42" s="51"/>
+      <c r="M42" s="51"/>
+      <c r="N42" s="51"/>
+      <c r="O42" s="51"/>
       <c r="P42" s="51"/>
       <c r="Q42" s="51"/>
       <c r="R42" s="51"/>
@@ -4046,9 +4069,9 @@
       <c r="AP42" s="43"/>
       <c r="AQ42" s="43"/>
       <c r="AR42" s="43"/>
-      <c r="AS42" s="107"/>
+      <c r="AS42" s="43"/>
       <c r="AT42" s="43"/>
-      <c r="AU42" s="43"/>
+      <c r="AU42" s="107"/>
       <c r="AV42" s="43"/>
       <c r="AW42" s="43"/>
       <c r="AX42" s="43"/>
@@ -4057,19 +4080,19 @@
     </row>
     <row r="43" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A43" s="92" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="B43" s="69">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C43" s="69">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D43" s="51"/>
       <c r="E43" s="51"/>
-      <c r="F43" s="51"/>
-      <c r="G43" s="51"/>
-      <c r="H43" s="51"/>
+      <c r="F43" s="93"/>
+      <c r="G43" s="93"/>
+      <c r="H43" s="94"/>
       <c r="I43" s="51"/>
       <c r="J43" s="51"/>
       <c r="K43" s="51"/>
@@ -4077,7 +4100,7 @@
       <c r="M43" s="51"/>
       <c r="N43" s="51"/>
       <c r="O43" s="51"/>
-      <c r="P43" s="93"/>
+      <c r="P43" s="51"/>
       <c r="Q43" s="51"/>
       <c r="R43" s="51"/>
       <c r="S43" s="51"/>
@@ -4098,9 +4121,9 @@
       <c r="AP43" s="43"/>
       <c r="AQ43" s="43"/>
       <c r="AR43" s="43"/>
-      <c r="AS43" s="107"/>
+      <c r="AS43" s="43"/>
       <c r="AT43" s="43"/>
-      <c r="AU43" s="43"/>
+      <c r="AU43" s="107"/>
       <c r="AV43" s="43"/>
       <c r="AW43" s="43"/>
       <c r="AX43" s="43"/>
@@ -4109,31 +4132,31 @@
     </row>
     <row r="44" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A44" s="92" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="B44" s="69">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C44" s="69">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D44" s="51"/>
       <c r="E44" s="51"/>
       <c r="F44" s="51"/>
       <c r="G44" s="51"/>
       <c r="H44" s="51"/>
-      <c r="I44" s="51"/>
-      <c r="J44" s="51"/>
-      <c r="K44" s="51"/>
-      <c r="L44" s="51"/>
-      <c r="M44" s="51"/>
-      <c r="N44" s="51"/>
-      <c r="O44" s="51"/>
+      <c r="I44" s="93"/>
+      <c r="J44" s="93"/>
+      <c r="K44" s="93"/>
+      <c r="L44" s="93"/>
+      <c r="M44" s="93"/>
+      <c r="N44" s="94"/>
+      <c r="O44" s="94"/>
       <c r="P44" s="51"/>
-      <c r="Q44" s="93"/>
-      <c r="R44" s="103"/>
-      <c r="S44" s="94"/>
-      <c r="T44" s="94"/>
+      <c r="Q44" s="51"/>
+      <c r="R44" s="51"/>
+      <c r="S44" s="51"/>
+      <c r="T44" s="51"/>
       <c r="U44" s="51"/>
       <c r="V44" s="51"/>
       <c r="W44" s="51"/>
@@ -4150,9 +4173,9 @@
       <c r="AP44" s="43"/>
       <c r="AQ44" s="43"/>
       <c r="AR44" s="43"/>
-      <c r="AS44" s="107"/>
+      <c r="AS44" s="43"/>
       <c r="AT44" s="43"/>
-      <c r="AU44" s="43"/>
+      <c r="AU44" s="107"/>
       <c r="AV44" s="43"/>
       <c r="AW44" s="43"/>
       <c r="AX44" s="43"/>
@@ -4161,13 +4184,13 @@
     </row>
     <row r="45" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A45" s="92" t="s">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="B45" s="69">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C45" s="69">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D45" s="51"/>
       <c r="E45" s="51"/>
@@ -4181,16 +4204,16 @@
       <c r="M45" s="51"/>
       <c r="N45" s="51"/>
       <c r="O45" s="51"/>
-      <c r="P45" s="51"/>
+      <c r="P45" s="93"/>
       <c r="Q45" s="51"/>
       <c r="R45" s="51"/>
       <c r="S45" s="51"/>
       <c r="T45" s="51"/>
-      <c r="U45" s="93"/>
-      <c r="V45" s="93"/>
-      <c r="W45" s="93"/>
-      <c r="X45" s="103"/>
-      <c r="Y45" s="94"/>
+      <c r="U45" s="51"/>
+      <c r="V45" s="51"/>
+      <c r="W45" s="51"/>
+      <c r="X45" s="51"/>
+      <c r="Y45" s="51"/>
       <c r="Z45" s="51"/>
       <c r="AA45" s="51"/>
       <c r="AB45" s="51"/>
@@ -4202,71 +4225,61 @@
       <c r="AP45" s="43"/>
       <c r="AQ45" s="43"/>
       <c r="AR45" s="43"/>
-      <c r="AS45" s="107"/>
+      <c r="AS45" s="43"/>
       <c r="AT45" s="43"/>
-      <c r="AU45" s="43"/>
+      <c r="AU45" s="107"/>
       <c r="AV45" s="43"/>
       <c r="AW45" s="43"/>
       <c r="AX45" s="43"/>
       <c r="AY45" s="43"/>
       <c r="AZ45" s="43"/>
     </row>
-    <row r="46" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46" s="95">
-        <f>SUM(B40:B45)</f>
-        <v>61</v>
-      </c>
-      <c r="C46" s="95">
-        <f>SUM(C40:C45)</f>
-        <v>29</v>
-      </c>
-      <c r="D46" s="96"/>
-      <c r="E46" s="96"/>
-      <c r="F46" s="96"/>
-      <c r="G46" s="96"/>
-      <c r="H46" s="96"/>
-      <c r="I46" s="96"/>
-      <c r="J46" s="96"/>
-      <c r="K46" s="96"/>
-      <c r="L46" s="96"/>
-      <c r="M46" s="96"/>
-      <c r="N46" s="96"/>
-      <c r="O46" s="96"/>
-      <c r="P46" s="96"/>
-      <c r="Q46" s="96"/>
-      <c r="R46" s="96"/>
-      <c r="S46" s="96"/>
-      <c r="T46" s="96"/>
-      <c r="U46" s="96"/>
-      <c r="V46" s="96"/>
-      <c r="W46" s="96"/>
-      <c r="X46" s="96"/>
-      <c r="Y46" s="96"/>
-      <c r="Z46" s="96"/>
-      <c r="AA46" s="96"/>
-      <c r="AB46" s="96"/>
-      <c r="AC46" s="96"/>
-      <c r="AD46" s="96"/>
-      <c r="AE46" s="96"/>
-      <c r="AF46" s="96"/>
-      <c r="AG46" s="96"/>
-      <c r="AH46" s="96"/>
-      <c r="AI46" s="96"/>
-      <c r="AJ46" s="96"/>
-      <c r="AK46" s="96"/>
-      <c r="AL46" s="96"/>
-      <c r="AM46" s="96"/>
-      <c r="AN46" s="96"/>
-      <c r="AO46" s="96"/>
-      <c r="AP46" s="96"/>
-      <c r="AQ46" s="96"/>
-      <c r="AR46" s="96"/>
-      <c r="AS46" s="108"/>
+    <row r="46" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A46" s="92" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="69">
+        <v>12</v>
+      </c>
+      <c r="C46" s="69">
+        <v>8</v>
+      </c>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="51"/>
+      <c r="I46" s="51"/>
+      <c r="J46" s="51"/>
+      <c r="K46" s="51"/>
+      <c r="L46" s="51"/>
+      <c r="M46" s="51"/>
+      <c r="N46" s="51"/>
+      <c r="O46" s="51"/>
+      <c r="P46" s="51"/>
+      <c r="Q46" s="93"/>
+      <c r="R46" s="93"/>
+      <c r="S46" s="93"/>
+      <c r="T46" s="94"/>
+      <c r="U46" s="51"/>
+      <c r="V46" s="51"/>
+      <c r="W46" s="51"/>
+      <c r="X46" s="51"/>
+      <c r="Y46" s="51"/>
+      <c r="Z46" s="51"/>
+      <c r="AA46" s="51"/>
+      <c r="AB46" s="51"/>
+      <c r="AC46" s="51"/>
+      <c r="AD46" s="51"/>
+      <c r="AE46" s="51"/>
+      <c r="AN46" s="43"/>
+      <c r="AO46" s="43"/>
+      <c r="AP46" s="43"/>
+      <c r="AQ46" s="43"/>
+      <c r="AR46" s="43"/>
+      <c r="AS46" s="43"/>
       <c r="AT46" s="43"/>
-      <c r="AU46" s="43"/>
+      <c r="AU46" s="107"/>
       <c r="AV46" s="43"/>
       <c r="AW46" s="43"/>
       <c r="AX46" s="43"/>
@@ -4274,99 +4287,113 @@
       <c r="AZ46" s="43"/>
     </row>
     <row r="47" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A47" s="98" t="s">
-        <v>32</v>
-      </c>
-      <c r="B47" s="88"/>
-      <c r="C47" s="88"/>
-      <c r="D47" s="60"/>
-      <c r="E47" s="60"/>
-      <c r="F47" s="60"/>
-      <c r="G47" s="60"/>
-      <c r="H47" s="60"/>
-      <c r="I47" s="60"/>
-      <c r="J47" s="60"/>
-      <c r="K47" s="60"/>
-      <c r="L47" s="60"/>
-      <c r="M47" s="60"/>
-      <c r="N47" s="60"/>
-      <c r="O47" s="60"/>
-      <c r="P47" s="60"/>
-      <c r="Q47" s="60"/>
-      <c r="R47" s="60"/>
-      <c r="S47" s="60"/>
-      <c r="T47" s="60"/>
-      <c r="U47" s="60"/>
-      <c r="V47" s="60"/>
-      <c r="W47" s="60"/>
-      <c r="X47" s="60"/>
-      <c r="Y47" s="60"/>
-      <c r="Z47" s="60"/>
-      <c r="AA47" s="60"/>
-      <c r="AB47" s="60"/>
-      <c r="AC47" s="60"/>
-      <c r="AD47" s="60"/>
-      <c r="AE47" s="60"/>
+      <c r="A47" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="69">
+        <v>15</v>
+      </c>
+      <c r="C47" s="69">
+        <v>12</v>
+      </c>
+      <c r="D47" s="51"/>
+      <c r="E47" s="51"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="51"/>
+      <c r="I47" s="51"/>
+      <c r="J47" s="51"/>
+      <c r="K47" s="51"/>
+      <c r="L47" s="51"/>
+      <c r="M47" s="51"/>
+      <c r="N47" s="51"/>
+      <c r="O47" s="51"/>
+      <c r="P47" s="51"/>
+      <c r="Q47" s="51"/>
+      <c r="R47" s="51"/>
+      <c r="S47" s="51"/>
+      <c r="T47" s="51"/>
+      <c r="U47" s="93"/>
+      <c r="V47" s="93"/>
+      <c r="W47" s="93"/>
+      <c r="X47" s="103"/>
+      <c r="Y47" s="94"/>
+      <c r="Z47" s="51"/>
+      <c r="AA47" s="51"/>
+      <c r="AB47" s="51"/>
+      <c r="AC47" s="51"/>
+      <c r="AD47" s="51"/>
+      <c r="AE47" s="51"/>
       <c r="AN47" s="43"/>
       <c r="AO47" s="43"/>
       <c r="AP47" s="43"/>
       <c r="AQ47" s="43"/>
       <c r="AR47" s="43"/>
-      <c r="AS47" s="107"/>
+      <c r="AS47" s="43"/>
       <c r="AT47" s="43"/>
-      <c r="AU47" s="43"/>
+      <c r="AU47" s="107"/>
       <c r="AV47" s="43"/>
       <c r="AW47" s="43"/>
       <c r="AX47" s="43"/>
       <c r="AY47" s="43"/>
       <c r="AZ47" s="43"/>
     </row>
-    <row r="48" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A48" s="92" t="s">
-        <v>41</v>
-      </c>
-      <c r="B48" s="69">
-        <v>2</v>
-      </c>
-      <c r="C48" s="69">
-        <v>2</v>
-      </c>
-      <c r="D48" s="51"/>
-      <c r="E48" s="93"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="51"/>
-      <c r="H48" s="51"/>
-      <c r="I48" s="51"/>
-      <c r="J48" s="51"/>
-      <c r="K48" s="51"/>
-      <c r="L48" s="51"/>
-      <c r="M48" s="51"/>
-      <c r="N48" s="51"/>
-      <c r="O48" s="51"/>
-      <c r="P48" s="51"/>
-      <c r="Q48" s="51"/>
-      <c r="R48" s="51"/>
-      <c r="S48" s="51"/>
-      <c r="T48" s="51"/>
-      <c r="U48" s="51"/>
-      <c r="V48" s="51"/>
-      <c r="W48" s="51"/>
-      <c r="X48" s="51"/>
-      <c r="Y48" s="51"/>
-      <c r="Z48" s="51"/>
-      <c r="AA48" s="51"/>
-      <c r="AB48" s="51"/>
-      <c r="AC48" s="51"/>
-      <c r="AD48" s="51"/>
-      <c r="AE48" s="51"/>
-      <c r="AN48" s="43"/>
-      <c r="AO48" s="43"/>
-      <c r="AP48" s="43"/>
-      <c r="AQ48" s="43"/>
-      <c r="AR48" s="43"/>
-      <c r="AS48" s="107"/>
-      <c r="AT48" s="43"/>
-      <c r="AU48" s="43"/>
+    <row r="48" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="95">
+        <f>SUM(B42:B47)</f>
+        <v>61</v>
+      </c>
+      <c r="C48" s="95">
+        <f>SUM(C42:C47)</f>
+        <v>49</v>
+      </c>
+      <c r="D48" s="96"/>
+      <c r="E48" s="96"/>
+      <c r="F48" s="96"/>
+      <c r="G48" s="96"/>
+      <c r="H48" s="96"/>
+      <c r="I48" s="96"/>
+      <c r="J48" s="96"/>
+      <c r="K48" s="96"/>
+      <c r="L48" s="96"/>
+      <c r="M48" s="96"/>
+      <c r="N48" s="96"/>
+      <c r="O48" s="96"/>
+      <c r="P48" s="96"/>
+      <c r="Q48" s="96"/>
+      <c r="R48" s="96"/>
+      <c r="S48" s="96"/>
+      <c r="T48" s="96"/>
+      <c r="U48" s="96"/>
+      <c r="V48" s="96"/>
+      <c r="W48" s="96"/>
+      <c r="X48" s="96"/>
+      <c r="Y48" s="96"/>
+      <c r="Z48" s="96"/>
+      <c r="AA48" s="96"/>
+      <c r="AB48" s="96"/>
+      <c r="AC48" s="96"/>
+      <c r="AD48" s="96"/>
+      <c r="AE48" s="96"/>
+      <c r="AF48" s="96"/>
+      <c r="AG48" s="96"/>
+      <c r="AH48" s="96"/>
+      <c r="AI48" s="96"/>
+      <c r="AJ48" s="96"/>
+      <c r="AK48" s="96"/>
+      <c r="AL48" s="96"/>
+      <c r="AM48" s="96"/>
+      <c r="AN48" s="96"/>
+      <c r="AO48" s="96"/>
+      <c r="AP48" s="96"/>
+      <c r="AQ48" s="96"/>
+      <c r="AR48" s="96"/>
+      <c r="AS48" s="96"/>
+      <c r="AT48" s="96"/>
+      <c r="AU48" s="108"/>
       <c r="AV48" s="43"/>
       <c r="AW48" s="43"/>
       <c r="AX48" s="43"/>
@@ -4374,51 +4401,47 @@
       <c r="AZ48" s="43"/>
     </row>
     <row r="49" spans="1:52" x14ac:dyDescent="0.25">
-      <c r="A49" s="92" t="s">
-        <v>33</v>
-      </c>
-      <c r="B49" s="69">
-        <v>5</v>
-      </c>
-      <c r="C49" s="69">
-        <v>1</v>
-      </c>
-      <c r="D49" s="51"/>
-      <c r="E49" s="51"/>
-      <c r="F49" s="93"/>
-      <c r="G49" s="103"/>
-      <c r="H49" s="94"/>
-      <c r="I49" s="51"/>
-      <c r="J49" s="51"/>
-      <c r="K49" s="51"/>
-      <c r="L49" s="51"/>
-      <c r="M49" s="51"/>
-      <c r="N49" s="51"/>
-      <c r="O49" s="51"/>
-      <c r="P49" s="51"/>
-      <c r="Q49" s="51"/>
-      <c r="R49" s="51"/>
-      <c r="S49" s="51"/>
-      <c r="T49" s="51"/>
-      <c r="U49" s="51"/>
-      <c r="V49" s="51"/>
-      <c r="W49" s="51"/>
-      <c r="X49" s="51"/>
-      <c r="Y49" s="51"/>
-      <c r="Z49" s="51"/>
-      <c r="AA49" s="51"/>
-      <c r="AB49" s="51"/>
-      <c r="AC49" s="51"/>
-      <c r="AD49" s="51"/>
-      <c r="AE49" s="51"/>
+      <c r="A49" s="98" t="s">
+        <v>32</v>
+      </c>
+      <c r="B49" s="88"/>
+      <c r="C49" s="88"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="60"/>
+      <c r="F49" s="60"/>
+      <c r="G49" s="60"/>
+      <c r="H49" s="60"/>
+      <c r="I49" s="60"/>
+      <c r="J49" s="60"/>
+      <c r="K49" s="60"/>
+      <c r="L49" s="60"/>
+      <c r="M49" s="60"/>
+      <c r="N49" s="60"/>
+      <c r="O49" s="60"/>
+      <c r="P49" s="60"/>
+      <c r="Q49" s="60"/>
+      <c r="R49" s="60"/>
+      <c r="S49" s="60"/>
+      <c r="T49" s="60"/>
+      <c r="U49" s="60"/>
+      <c r="V49" s="60"/>
+      <c r="W49" s="60"/>
+      <c r="X49" s="60"/>
+      <c r="Y49" s="60"/>
+      <c r="Z49" s="60"/>
+      <c r="AA49" s="60"/>
+      <c r="AB49" s="60"/>
+      <c r="AC49" s="60"/>
+      <c r="AD49" s="60"/>
+      <c r="AE49" s="60"/>
       <c r="AN49" s="43"/>
       <c r="AO49" s="43"/>
       <c r="AP49" s="43"/>
       <c r="AQ49" s="43"/>
       <c r="AR49" s="43"/>
-      <c r="AS49" s="107"/>
+      <c r="AS49" s="43"/>
       <c r="AT49" s="43"/>
-      <c r="AU49" s="43"/>
+      <c r="AU49" s="107"/>
       <c r="AV49" s="43"/>
       <c r="AW49" s="43"/>
       <c r="AX49" s="43"/>
@@ -4427,21 +4450,21 @@
     </row>
     <row r="50" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A50" s="92" t="s">
-        <v>91</v>
+        <v>41</v>
       </c>
       <c r="B50" s="69">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C50" s="69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D50" s="51"/>
-      <c r="E50" s="51"/>
+      <c r="E50" s="93"/>
       <c r="F50" s="51"/>
       <c r="G50" s="51"/>
       <c r="H50" s="51"/>
-      <c r="I50" s="93"/>
-      <c r="J50" s="103"/>
+      <c r="I50" s="51"/>
+      <c r="J50" s="51"/>
       <c r="K50" s="51"/>
       <c r="L50" s="51"/>
       <c r="M50" s="51"/>
@@ -4468,9 +4491,9 @@
       <c r="AP50" s="43"/>
       <c r="AQ50" s="43"/>
       <c r="AR50" s="43"/>
-      <c r="AS50" s="107"/>
+      <c r="AS50" s="43"/>
       <c r="AT50" s="43"/>
-      <c r="AU50" s="43"/>
+      <c r="AU50" s="107"/>
       <c r="AV50" s="43"/>
       <c r="AW50" s="43"/>
       <c r="AX50" s="43"/>
@@ -4479,23 +4502,23 @@
     </row>
     <row r="51" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A51" s="92" t="s">
-        <v>92</v>
+        <v>33</v>
       </c>
       <c r="B51" s="69">
         <v>5</v>
       </c>
       <c r="C51" s="69">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D51" s="51"/>
       <c r="E51" s="51"/>
-      <c r="F51" s="51"/>
-      <c r="G51" s="51"/>
+      <c r="F51" s="93"/>
+      <c r="G51" s="103"/>
       <c r="H51" s="51"/>
       <c r="I51" s="51"/>
       <c r="J51" s="51"/>
-      <c r="K51" s="93"/>
-      <c r="L51" s="93"/>
+      <c r="K51" s="51"/>
+      <c r="L51" s="51"/>
       <c r="M51" s="51"/>
       <c r="N51" s="51"/>
       <c r="O51" s="51"/>
@@ -4520,9 +4543,9 @@
       <c r="AP51" s="43"/>
       <c r="AQ51" s="43"/>
       <c r="AR51" s="43"/>
-      <c r="AS51" s="107"/>
+      <c r="AS51" s="43"/>
       <c r="AT51" s="43"/>
-      <c r="AU51" s="43"/>
+      <c r="AU51" s="107"/>
       <c r="AV51" s="43"/>
       <c r="AW51" s="43"/>
       <c r="AX51" s="43"/>
@@ -4531,20 +4554,20 @@
     </row>
     <row r="52" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A52" s="92" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="B52" s="69">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C52" s="69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52" s="51"/>
       <c r="E52" s="51"/>
       <c r="F52" s="51"/>
       <c r="G52" s="51"/>
-      <c r="H52" s="51"/>
-      <c r="I52" s="51"/>
+      <c r="H52" s="93"/>
+      <c r="I52" s="103"/>
       <c r="J52" s="51"/>
       <c r="K52" s="51"/>
       <c r="L52" s="51"/>
@@ -4572,9 +4595,9 @@
       <c r="AP52" s="43"/>
       <c r="AQ52" s="43"/>
       <c r="AR52" s="43"/>
-      <c r="AS52" s="107"/>
+      <c r="AS52" s="43"/>
       <c r="AT52" s="43"/>
-      <c r="AU52" s="43"/>
+      <c r="AU52" s="107"/>
       <c r="AV52" s="43"/>
       <c r="AW52" s="43"/>
       <c r="AX52" s="43"/>
@@ -4583,7 +4606,7 @@
     </row>
     <row r="53" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A53" s="92" t="s">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="B53" s="69">
         <v>5</v>
@@ -4597,11 +4620,11 @@
       <c r="G53" s="51"/>
       <c r="H53" s="51"/>
       <c r="I53" s="51"/>
-      <c r="J53" s="51"/>
-      <c r="K53" s="51"/>
+      <c r="J53" s="93"/>
+      <c r="K53" s="103"/>
       <c r="L53" s="51"/>
-      <c r="M53" s="93"/>
-      <c r="N53" s="93"/>
+      <c r="M53" s="51"/>
+      <c r="N53" s="51"/>
       <c r="O53" s="51"/>
       <c r="P53" s="51"/>
       <c r="Q53" s="51"/>
@@ -4624,117 +4647,105 @@
       <c r="AP53" s="43"/>
       <c r="AQ53" s="43"/>
       <c r="AR53" s="43"/>
-      <c r="AS53" s="107"/>
+      <c r="AS53" s="43"/>
       <c r="AT53" s="43"/>
-      <c r="AU53" s="43"/>
+      <c r="AU53" s="107"/>
       <c r="AV53" s="43"/>
       <c r="AW53" s="43"/>
       <c r="AX53" s="43"/>
       <c r="AY53" s="43"/>
       <c r="AZ53" s="43"/>
     </row>
-    <row r="54" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="B54" s="95">
-        <f>SUM(B48:B53)</f>
-        <v>22</v>
-      </c>
-      <c r="C54" s="95">
-        <f>SUM(C48:C53)</f>
-        <v>12</v>
-      </c>
-      <c r="D54" s="96"/>
-      <c r="E54" s="96"/>
-      <c r="F54" s="96"/>
-      <c r="G54" s="96"/>
-      <c r="H54" s="96"/>
-      <c r="I54" s="96"/>
-      <c r="J54" s="96"/>
-      <c r="K54" s="96"/>
-      <c r="L54" s="96"/>
-      <c r="M54" s="96"/>
-      <c r="N54" s="96"/>
-      <c r="O54" s="96"/>
-      <c r="P54" s="96"/>
-      <c r="Q54" s="96"/>
-      <c r="R54" s="96"/>
-      <c r="S54" s="96"/>
-      <c r="T54" s="96"/>
-      <c r="U54" s="96"/>
-      <c r="V54" s="96"/>
-      <c r="W54" s="96"/>
-      <c r="X54" s="96"/>
-      <c r="Y54" s="96"/>
-      <c r="Z54" s="96"/>
-      <c r="AA54" s="96"/>
-      <c r="AB54" s="96"/>
-      <c r="AC54" s="96"/>
-      <c r="AD54" s="96"/>
-      <c r="AE54" s="96"/>
-      <c r="AF54" s="96"/>
-      <c r="AG54" s="96"/>
-      <c r="AH54" s="96"/>
-      <c r="AI54" s="96"/>
-      <c r="AJ54" s="96"/>
-      <c r="AK54" s="96"/>
-      <c r="AL54" s="96"/>
-      <c r="AM54" s="96"/>
-      <c r="AN54" s="96"/>
-      <c r="AO54" s="96"/>
-      <c r="AP54" s="96"/>
-      <c r="AQ54" s="96"/>
-      <c r="AR54" s="96"/>
-      <c r="AS54" s="108"/>
+    <row r="54" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A54" s="92" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="69">
+        <v>0</v>
+      </c>
+      <c r="C54" s="69">
+        <v>0</v>
+      </c>
+      <c r="D54" s="51"/>
+      <c r="E54" s="51"/>
+      <c r="F54" s="51"/>
+      <c r="G54" s="51"/>
+      <c r="H54" s="51"/>
+      <c r="I54" s="51"/>
+      <c r="J54" s="51"/>
+      <c r="K54" s="51"/>
+      <c r="L54" s="51"/>
+      <c r="M54" s="51"/>
+      <c r="N54" s="51"/>
+      <c r="O54" s="51"/>
+      <c r="P54" s="51"/>
+      <c r="Q54" s="51"/>
+      <c r="R54" s="51"/>
+      <c r="S54" s="51"/>
+      <c r="T54" s="51"/>
+      <c r="U54" s="51"/>
+      <c r="V54" s="51"/>
+      <c r="W54" s="51"/>
+      <c r="X54" s="51"/>
+      <c r="Y54" s="51"/>
+      <c r="Z54" s="51"/>
+      <c r="AA54" s="51"/>
+      <c r="AB54" s="51"/>
+      <c r="AC54" s="51"/>
+      <c r="AD54" s="51"/>
+      <c r="AE54" s="51"/>
+      <c r="AN54" s="43"/>
+      <c r="AO54" s="43"/>
+      <c r="AP54" s="43"/>
+      <c r="AQ54" s="43"/>
+      <c r="AR54" s="43"/>
+      <c r="AS54" s="43"/>
       <c r="AT54" s="43"/>
-      <c r="AU54" s="43"/>
+      <c r="AU54" s="107"/>
       <c r="AV54" s="43"/>
       <c r="AW54" s="43"/>
       <c r="AX54" s="43"/>
       <c r="AY54" s="43"/>
       <c r="AZ54" s="43"/>
     </row>
-    <row r="55" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="86" t="s">
+    <row r="55" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A55" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="69">
         <v>5</v>
       </c>
-      <c r="B55" s="86">
-        <f>SUM(B10,B20,B54,B29,B38,B46)</f>
-        <v>291</v>
-      </c>
-      <c r="C55" s="86">
-        <f>SUM(C29,C38,C46,C54,C10,C20)</f>
-        <v>200</v>
-      </c>
-      <c r="D55" s="43"/>
-      <c r="E55" s="43"/>
-      <c r="F55" s="43"/>
-      <c r="G55" s="43"/>
-      <c r="H55" s="43"/>
-      <c r="I55" s="43"/>
-      <c r="J55" s="43"/>
-      <c r="K55" s="43"/>
-      <c r="L55" s="43"/>
-      <c r="M55" s="43"/>
-      <c r="N55" s="43"/>
-      <c r="O55" s="43"/>
-      <c r="P55" s="43"/>
-      <c r="Q55" s="43"/>
-      <c r="R55" s="43"/>
-      <c r="S55" s="43"/>
-      <c r="T55" s="43"/>
-      <c r="U55" s="43"/>
-      <c r="V55" s="43"/>
-      <c r="W55" s="43"/>
-      <c r="X55" s="43"/>
-      <c r="Y55" s="43"/>
-      <c r="Z55" s="43"/>
-      <c r="AA55" s="43"/>
-      <c r="AB55" s="43"/>
-      <c r="AC55" s="43"/>
-      <c r="AD55" s="43"/>
-      <c r="AE55" s="43"/>
+      <c r="C55" s="69">
+        <v>4</v>
+      </c>
+      <c r="D55" s="51"/>
+      <c r="E55" s="51"/>
+      <c r="F55" s="51"/>
+      <c r="G55" s="51"/>
+      <c r="H55" s="51"/>
+      <c r="I55" s="51"/>
+      <c r="J55" s="51"/>
+      <c r="K55" s="51"/>
+      <c r="L55" s="93"/>
+      <c r="M55" s="93"/>
+      <c r="N55" s="51"/>
+      <c r="O55" s="51"/>
+      <c r="P55" s="51"/>
+      <c r="Q55" s="51"/>
+      <c r="R55" s="51"/>
+      <c r="S55" s="51"/>
+      <c r="T55" s="51"/>
+      <c r="U55" s="51"/>
+      <c r="V55" s="51"/>
+      <c r="W55" s="51"/>
+      <c r="X55" s="51"/>
+      <c r="Y55" s="51"/>
+      <c r="Z55" s="51"/>
+      <c r="AA55" s="51"/>
+      <c r="AB55" s="51"/>
+      <c r="AC55" s="51"/>
+      <c r="AD55" s="51"/>
+      <c r="AE55" s="51"/>
       <c r="AN55" s="43"/>
       <c r="AO55" s="43"/>
       <c r="AP55" s="43"/>
@@ -4742,54 +4753,81 @@
       <c r="AR55" s="43"/>
       <c r="AS55" s="43"/>
       <c r="AT55" s="43"/>
-      <c r="AU55" s="43"/>
+      <c r="AU55" s="107"/>
       <c r="AV55" s="43"/>
       <c r="AW55" s="43"/>
       <c r="AX55" s="43"/>
       <c r="AY55" s="43"/>
     </row>
     <row r="56" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="62" t="s">
-        <v>6</v>
-      </c>
-      <c r="B56" s="63">
-        <f>B55*100</f>
-        <v>29100</v>
-      </c>
-      <c r="C56" s="63">
-        <f>C55*100</f>
-        <v>20000</v>
-      </c>
-      <c r="D56" s="43"/>
-      <c r="E56" s="43"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
-      <c r="H56" s="43"/>
-      <c r="I56" s="43"/>
-      <c r="J56" s="43"/>
-      <c r="K56" s="43"/>
-      <c r="L56" s="43"/>
-      <c r="M56" s="43"/>
-      <c r="N56" s="43"/>
-      <c r="O56" s="43"/>
-      <c r="P56" s="43"/>
-      <c r="Q56" s="43"/>
-      <c r="R56" s="43"/>
-      <c r="S56" s="43"/>
-      <c r="T56" s="43"/>
-      <c r="U56" s="43"/>
-      <c r="V56" s="43"/>
-      <c r="W56" s="43"/>
-      <c r="X56" s="43"/>
-      <c r="Y56" s="43"/>
-      <c r="Z56" s="43"/>
-      <c r="AA56" s="43"/>
-      <c r="AB56" s="43"/>
-      <c r="AC56" s="43"/>
-      <c r="AD56" s="43"/>
-      <c r="AE56" s="43"/>
-    </row>
-    <row r="57" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="A56" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56" s="95">
+        <f>SUM(B50:B55)</f>
+        <v>22</v>
+      </c>
+      <c r="C56" s="95">
+        <f>SUM(C50:C55)</f>
+        <v>12</v>
+      </c>
+      <c r="D56" s="96"/>
+      <c r="E56" s="96"/>
+      <c r="F56" s="96"/>
+      <c r="G56" s="96"/>
+      <c r="H56" s="96"/>
+      <c r="I56" s="96"/>
+      <c r="J56" s="96"/>
+      <c r="K56" s="96"/>
+      <c r="L56" s="96"/>
+      <c r="M56" s="96"/>
+      <c r="N56" s="96"/>
+      <c r="O56" s="96"/>
+      <c r="P56" s="96"/>
+      <c r="Q56" s="96"/>
+      <c r="R56" s="96"/>
+      <c r="S56" s="96"/>
+      <c r="T56" s="96"/>
+      <c r="U56" s="96"/>
+      <c r="V56" s="96"/>
+      <c r="W56" s="96"/>
+      <c r="X56" s="96"/>
+      <c r="Y56" s="96"/>
+      <c r="Z56" s="96"/>
+      <c r="AA56" s="96"/>
+      <c r="AB56" s="96"/>
+      <c r="AC56" s="96"/>
+      <c r="AD56" s="96"/>
+      <c r="AE56" s="96"/>
+      <c r="AF56" s="96"/>
+      <c r="AG56" s="96"/>
+      <c r="AH56" s="96"/>
+      <c r="AI56" s="96"/>
+      <c r="AJ56" s="96"/>
+      <c r="AK56" s="96"/>
+      <c r="AL56" s="96"/>
+      <c r="AM56" s="96"/>
+      <c r="AN56" s="96"/>
+      <c r="AO56" s="96"/>
+      <c r="AP56" s="96"/>
+      <c r="AQ56" s="96"/>
+      <c r="AR56" s="96"/>
+      <c r="AS56" s="96"/>
+      <c r="AT56" s="96"/>
+      <c r="AU56" s="108"/>
+    </row>
+    <row r="57" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="86" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" s="86">
+        <f>SUM(B11,B22,B56,B31,B40,B48)</f>
+        <v>300</v>
+      </c>
+      <c r="C57" s="86">
+        <f>SUM(C31,C40,C48,C56,C11,C22)</f>
+        <v>255</v>
+      </c>
       <c r="D57" s="43"/>
       <c r="E57" s="43"/>
       <c r="F57" s="43"/>
@@ -4816,8 +4854,27 @@
       <c r="AA57" s="43"/>
       <c r="AB57" s="43"/>
       <c r="AC57" s="43"/>
-    </row>
-    <row r="58" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AD57" s="43"/>
+      <c r="AE57" s="43"/>
+      <c r="AN57" s="43"/>
+      <c r="AO57" s="43"/>
+      <c r="AP57" s="43"/>
+      <c r="AQ57" s="43"/>
+      <c r="AR57" s="43"/>
+      <c r="AS57" s="43"/>
+    </row>
+    <row r="58" spans="1:52" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="63">
+        <f>B57*100</f>
+        <v>30000</v>
+      </c>
+      <c r="C58" s="63">
+        <f>C57*100</f>
+        <v>25500</v>
+      </c>
       <c r="D58" s="43"/>
       <c r="E58" s="43"/>
       <c r="F58" s="43"/>
@@ -4844,6 +4901,8 @@
       <c r="AA58" s="43"/>
       <c r="AB58" s="43"/>
       <c r="AC58" s="43"/>
+      <c r="AD58" s="43"/>
+      <c r="AE58" s="43"/>
     </row>
     <row r="59" spans="1:52" x14ac:dyDescent="0.25">
       <c r="D59" s="43"/>
@@ -5081,9 +5140,8 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5123,7 +5181,7 @@
         <v>95</v>
       </c>
       <c r="K1" s="80" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="L1" s="81" t="s">
         <v>38</v>
@@ -5159,7 +5217,7 @@
         <v>94</v>
       </c>
       <c r="K2" s="67" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="L2" s="82" t="s">
         <v>39</v>
@@ -5195,7 +5253,7 @@
         <v>3</v>
       </c>
       <c r="K3" s="66">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L3" s="83">
         <v>0</v>
@@ -5207,7 +5265,7 @@
       </c>
       <c r="B4" s="70">
         <f t="shared" ref="B4:B9" si="0">SUMIF(C4:L4,A$12,C$3:Z$3)</f>
-        <v>16.5</v>
+        <v>18.5</v>
       </c>
       <c r="C4" s="68" t="s">
         <v>12</v>
@@ -5233,7 +5291,9 @@
       <c r="J4" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="68"/>
+      <c r="K4" s="68" t="s">
+        <v>12</v>
+      </c>
       <c r="L4" s="84"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5242,7 +5302,7 @@
       </c>
       <c r="B5" s="70">
         <f t="shared" si="0"/>
-        <v>16.5</v>
+        <v>18.5</v>
       </c>
       <c r="C5" s="68" t="s">
         <v>12</v>
@@ -5268,7 +5328,9 @@
       <c r="J5" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="68"/>
+      <c r="K5" s="68" t="s">
+        <v>12</v>
+      </c>
       <c r="L5" s="84"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5277,7 +5339,7 @@
       </c>
       <c r="B6" s="70">
         <f t="shared" si="0"/>
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
       <c r="C6" s="68" t="s">
         <v>12</v>
@@ -5299,7 +5361,9 @@
         <v>12</v>
       </c>
       <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
+      <c r="K6" s="68" t="s">
+        <v>12</v>
+      </c>
       <c r="L6" s="84"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5308,7 +5372,7 @@
       </c>
       <c r="B7" s="70">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" s="68"/>
       <c r="D7" s="68" t="s">
@@ -5332,7 +5396,9 @@
       <c r="J7" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="68"/>
+      <c r="K7" s="68" t="s">
+        <v>12</v>
+      </c>
       <c r="L7" s="84"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5341,7 +5407,7 @@
       </c>
       <c r="B8" s="70">
         <f t="shared" si="0"/>
-        <v>9.5</v>
+        <v>11.5</v>
       </c>
       <c r="C8" s="68" t="s">
         <v>12</v>
@@ -5361,7 +5427,9 @@
       </c>
       <c r="I8" s="69"/>
       <c r="J8" s="68"/>
-      <c r="K8" s="68"/>
+      <c r="K8" s="68" t="s">
+        <v>12</v>
+      </c>
       <c r="L8" s="84"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5395,7 +5463,7 @@
       </c>
       <c r="B10" s="64">
         <f>SUM(B4:B9)</f>
-        <v>74.5</v>
+        <v>84.5</v>
       </c>
       <c r="C10" s="64">
         <f t="shared" ref="C10:L10" si="1">COUNTIF(C4:C9,"*ü*") * C3</f>
@@ -5431,7 +5499,7 @@
       </c>
       <c r="K10" s="64">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L10" s="64">
         <f t="shared" si="1"/>
@@ -5460,7 +5528,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="F45" sqref="F45"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>